<commit_message>
less corrected KwH from therms
</commit_message>
<xml_diff>
--- a/output/250812_all_costs.xlsx
+++ b/output/250812_all_costs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ischillebeeckx/Development/solar/output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F156844A-BC97-7649-8DE2-482D7D0F2970}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E6F755B-6EC1-4944-B69B-04B7C8B85D46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9460" yWindow="3360" windowWidth="30000" windowHeight="17440" xr2:uid="{26FF52C5-725B-6344-B119-F4C9063B9FBA}"/>
+    <workbookView xWindow="5780" yWindow="3380" windowWidth="30000" windowHeight="17440" xr2:uid="{26FF52C5-725B-6344-B119-F4C9063B9FBA}"/>
   </bookViews>
   <sheets>
     <sheet name="250812_all_costs" sheetId="1" r:id="rId1"/>
@@ -94,9 +94,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0%"/>
   </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
@@ -588,14 +589,16 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="2" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="21" builtinId="30" customBuiltin="1"/>
@@ -976,11 +979,13 @@
   <dimension ref="A1:AC37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="7" max="8" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="14.1640625" customWidth="1"/>
     <col min="23" max="24" width="20" bestFit="1" customWidth="1"/>
     <col min="27" max="29" width="15.83203125" bestFit="1" customWidth="1"/>
@@ -1072,712 +1077,712 @@
       <c r="A3">
         <v>0</v>
       </c>
-      <c r="B3">
-        <v>348.50498370051798</v>
-      </c>
-      <c r="C3">
-        <v>231.30272913532801</v>
-      </c>
-      <c r="D3">
-        <v>152.744071364826</v>
+      <c r="B3" s="1">
+        <v>206.432433</v>
+      </c>
+      <c r="C3" s="1">
+        <v>122.29416399999999</v>
+      </c>
+      <c r="D3" s="1">
+        <v>49.727231000000003</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="7">
         <f>$B$1*$B$32+$B$34*G$2</f>
-        <v>25000</v>
-      </c>
-      <c r="H3">
+        <v>23722</v>
+      </c>
+      <c r="H3" s="7">
         <f t="shared" ref="H3:I3" si="0">$B$1*$B$32+$B$34*H$2</f>
-        <v>26200</v>
-      </c>
-      <c r="I3">
+        <v>25538</v>
+      </c>
+      <c r="I3" s="7">
         <f t="shared" si="0"/>
-        <v>27280</v>
+        <v>27172.400000000001</v>
       </c>
       <c r="K3">
         <v>0</v>
       </c>
-      <c r="L3" s="2">
+      <c r="L3" s="6">
         <f>($B$35-B3)/G3</f>
-        <v>6.0819800651979276E-2</v>
-      </c>
-      <c r="M3" s="2">
+        <v>7.0085472009105476E-2</v>
+      </c>
+      <c r="M3" s="6">
         <f t="shared" ref="M3:N10" si="1">($B$35-C3)/H3</f>
-        <v>6.250752942231573E-2</v>
-      </c>
-      <c r="N3" s="2">
+        <v>6.8396344114652674E-2</v>
+      </c>
+      <c r="N3" s="6">
         <f t="shared" si="1"/>
-        <v>6.2912607354661809E-2</v>
+        <v>6.6952965840337983E-2</v>
       </c>
       <c r="P3">
         <v>0</v>
       </c>
       <c r="Q3" s="4">
         <f>LN(1+(G3*$B$36/($B$35-B3)))/LN(1+$B$36)</f>
-        <v>11.828569739955233</v>
+        <v>10.654313527892731</v>
       </c>
       <c r="R3" s="4">
         <f t="shared" ref="R3:S10" si="2">LN(1+(H3*$B$36/($B$35-C3)))/LN(1+$B$36)</f>
-        <v>11.595088333446929</v>
+        <v>10.850116863467074</v>
       </c>
       <c r="S3" s="4">
         <f t="shared" si="2"/>
-        <v>11.540464152725319</v>
+        <v>11.023418149500952</v>
       </c>
       <c r="U3">
         <v>0</v>
       </c>
-      <c r="V3" s="6" cm="1">
+      <c r="V3" s="5" cm="1">
         <f t="array" ref="V3">SUMPRODUCT(($B$35-B3) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G3</f>
-        <v>10122.60190984363</v>
-      </c>
-      <c r="W3" s="6" cm="1">
+        <v>14682.399999991096</v>
+      </c>
+      <c r="W3" s="5" cm="1">
         <f t="array" ref="W3">SUMPRODUCT(($B$35-C3) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H3</f>
-        <v>11629.909783859388</v>
-      </c>
-      <c r="X3" s="6" cm="1">
+        <v>14809.947920761311</v>
+      </c>
+      <c r="X3" s="5" cm="1">
         <f t="array" ref="X3">SUMPRODUCT(($B$35-D3) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I3</f>
-        <v>12364.57174188421</v>
+        <v>14851.804319010029</v>
       </c>
       <c r="Z3">
         <v>0</v>
       </c>
-      <c r="AA3" s="6" cm="1">
+      <c r="AA3" s="5" cm="1">
         <f t="array" ref="AA3">SUMPRODUCT(($B$35-B3) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G3</f>
-        <v>57255.817563480494</v>
-      </c>
-      <c r="AB3" s="6" cm="1">
+        <v>66219.665715513111</v>
+      </c>
+      <c r="AB3" s="5" cm="1">
         <f t="array" ref="AB3">SUMPRODUCT(($B$35-C3) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H3</f>
-        <v>62396.231156552094</v>
-      </c>
-      <c r="AC3" s="6" cm="1">
+        <v>68955.382117592977</v>
+      </c>
+      <c r="AC3" s="5" cm="1">
         <f t="array" ref="AC3">SUMPRODUCT(($B$35-D3) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I3</f>
-        <v>65566.101463479557</v>
+        <v>71246.711789839144</v>
       </c>
     </row>
     <row r="4" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>10</v>
       </c>
-      <c r="B4">
-        <v>284.14190411602601</v>
-      </c>
-      <c r="C4">
-        <v>165.00704467265601</v>
-      </c>
-      <c r="D4">
-        <v>81.205408724010297</v>
+      <c r="B4" s="1">
+        <v>153.46873099999999</v>
+      </c>
+      <c r="C4" s="1">
+        <v>59.969808499999999</v>
+      </c>
+      <c r="D4" s="1">
+        <v>-12.201634</v>
       </c>
       <c r="F4">
         <v>10</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="7">
         <f t="shared" ref="G4:I10" si="3">$B$1*$B$32+$B$34*G$2</f>
-        <v>25000</v>
-      </c>
-      <c r="H4">
+        <v>23722</v>
+      </c>
+      <c r="H4" s="7">
         <f t="shared" si="3"/>
-        <v>26200</v>
-      </c>
-      <c r="I4">
+        <v>25538</v>
+      </c>
+      <c r="I4" s="7">
         <f t="shared" si="3"/>
-        <v>27280</v>
+        <v>27172.400000000001</v>
       </c>
       <c r="K4">
         <v>10</v>
       </c>
-      <c r="L4" s="2">
+      <c r="L4" s="6">
         <f t="shared" ref="L4:L10" si="4">($B$35-B4)/G4</f>
-        <v>6.3394323835358951E-2</v>
-      </c>
-      <c r="M4" s="2">
+        <v>7.2318154835174106E-2</v>
+      </c>
+      <c r="M4" s="6">
         <f t="shared" si="1"/>
-        <v>6.5037899058295573E-2</v>
-      </c>
-      <c r="N4" s="2">
+        <v>7.0836799729814395E-2</v>
+      </c>
+      <c r="N4" s="6">
         <f t="shared" si="1"/>
-        <v>6.5534992348826607E-2</v>
+        <v>6.9232074973134494E-2</v>
       </c>
       <c r="P4">
         <v>10</v>
       </c>
       <c r="Q4" s="4">
         <f t="shared" ref="Q4:Q10" si="5">LN(1+(G4*$B$36/($B$35-B4)))/LN(1+$B$36)</f>
-        <v>11.476195421693886</v>
+        <v>10.406404648904884</v>
       </c>
       <c r="R4" s="4">
         <f t="shared" si="2"/>
-        <v>11.262385412408321</v>
+        <v>10.569540952598446</v>
       </c>
       <c r="S4" s="4">
         <f t="shared" si="2"/>
-        <v>11.199332909607907</v>
+        <v>10.752319673295499</v>
       </c>
       <c r="U4">
         <v>10</v>
       </c>
-      <c r="V4" s="6" cm="1">
+      <c r="V4" s="5" cm="1">
         <f t="array" ref="V4">SUMPRODUCT(($B$35-B4) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G4</f>
-        <v>11609.353788478154</v>
-      </c>
-      <c r="W4" s="6" cm="1">
+        <v>15905.832501299068</v>
+      </c>
+      <c r="W4" s="5" cm="1">
         <f t="array" ref="W4">SUMPRODUCT(($B$35-C4) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H4</f>
-        <v>13161.303776448716</v>
-      </c>
-      <c r="X4" s="6" cm="1">
+        <v>16249.606389910092</v>
+      </c>
+      <c r="X4" s="5" cm="1">
         <f t="array" ref="X4">SUMPRODUCT(($B$35-D4) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I4</f>
-        <v>14017.075658148984</v>
+        <v>16282.327174268787</v>
       </c>
       <c r="Z4">
         <v>10</v>
       </c>
-      <c r="AA4" s="6" cm="1">
+      <c r="AA4" s="5" cm="1">
         <f t="array" ref="AA4">SUMPRODUCT(($B$35-B4) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G4</f>
-        <v>60737.734751877884</v>
-      </c>
-      <c r="AB4" s="6" cm="1">
+        <v>69084.898789279687</v>
+      </c>
+      <c r="AB4" s="5" cm="1">
         <f t="array" ref="AB4">SUMPRODUCT(($B$35-C4) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H4</f>
-        <v>65982.698503008374</v>
-      </c>
-      <c r="AC4" s="6" cm="1">
+        <v>72327.008305652605</v>
+      </c>
+      <c r="AC4" s="5" cm="1">
         <f t="array" ref="AC4">SUMPRODUCT(($B$35-D4) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I4</f>
-        <v>69436.203712969116</v>
+        <v>74596.942712496792</v>
       </c>
     </row>
     <row r="5" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>20</v>
       </c>
-      <c r="B5">
-        <v>240.69839149606</v>
-      </c>
-      <c r="C5">
-        <v>117.70516472256099</v>
-      </c>
-      <c r="D5">
-        <v>39.352896438821404</v>
+      <c r="B5" s="1">
+        <v>113.480777</v>
+      </c>
+      <c r="C5" s="1">
+        <v>21.446580399999998</v>
+      </c>
+      <c r="D5" s="1">
+        <v>-40.694122999999998</v>
       </c>
       <c r="F5">
         <v>20</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="7">
         <f t="shared" si="3"/>
-        <v>25000</v>
-      </c>
-      <c r="H5">
+        <v>23722</v>
+      </c>
+      <c r="H5" s="7">
         <f t="shared" si="3"/>
-        <v>26200</v>
-      </c>
-      <c r="I5">
+        <v>25538</v>
+      </c>
+      <c r="I5" s="7">
         <f t="shared" si="3"/>
-        <v>27280</v>
+        <v>27172.400000000001</v>
       </c>
       <c r="K5">
         <v>20</v>
       </c>
-      <c r="L5" s="2">
+      <c r="L5" s="6">
         <f t="shared" si="4"/>
-        <v>6.51320643401576E-2</v>
-      </c>
-      <c r="M5" s="2">
+        <v>7.4003845502065596E-2</v>
+      </c>
+      <c r="M5" s="6">
         <f t="shared" si="1"/>
-        <v>6.6843314323566369E-2</v>
-      </c>
-      <c r="N5" s="2">
+        <v>7.2345266645782752E-2</v>
+      </c>
+      <c r="N5" s="6">
         <f t="shared" si="1"/>
-        <v>6.7069175350483082E-2</v>
+        <v>7.0280656953379164E-2</v>
       </c>
       <c r="P5">
         <v>20</v>
       </c>
       <c r="Q5" s="4">
         <f t="shared" si="5"/>
-        <v>11.250384938900833</v>
+        <v>10.226956859008041</v>
       </c>
       <c r="R5" s="4">
         <f t="shared" si="2"/>
-        <v>11.03681765914342</v>
+        <v>10.403467218156322</v>
       </c>
       <c r="S5" s="4">
         <f t="shared" si="2"/>
-        <v>11.009253884163872</v>
+        <v>10.632156252115085</v>
       </c>
       <c r="U5">
         <v>20</v>
       </c>
-      <c r="V5" s="6" cm="1">
+      <c r="V5" s="5" cm="1">
         <f t="array" ref="V5">SUMPRODUCT(($B$35-B5) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G5</f>
-        <v>12612.87513051444</v>
-      </c>
-      <c r="W5" s="6" cm="1">
+        <v>16829.532332258925</v>
+      </c>
+      <c r="W5" s="5" cm="1">
         <f t="array" ref="W5">SUMPRODUCT(($B$35-C5) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H5</f>
-        <v>14253.951290097117</v>
-      </c>
-      <c r="X5" s="6" cm="1">
+        <v>17139.471854994852</v>
+      </c>
+      <c r="X5" s="5" cm="1">
         <f t="array" ref="X5">SUMPRODUCT(($B$35-D5) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I5</f>
-        <v>14983.845764043232</v>
+        <v>16940.488061243042</v>
       </c>
       <c r="Z5">
         <v>20</v>
       </c>
-      <c r="AA5" s="6" cm="1">
+      <c r="AA5" s="5" cm="1">
         <f t="array" ref="AA5">SUMPRODUCT(($B$35-B5) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G5</f>
-        <v>63087.944131111319</v>
-      </c>
-      <c r="AB5" s="6" cm="1">
+        <v>71248.169180632933</v>
+      </c>
+      <c r="AB5" s="5" cm="1">
         <f t="array" ref="AB5">SUMPRODUCT(($B$35-C5) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H5</f>
-        <v>68541.638036433549</v>
-      </c>
-      <c r="AC5" s="6" cm="1">
+        <v>74411.039879963137</v>
+      </c>
+      <c r="AC5" s="5" cm="1">
         <f t="array" ref="AC5">SUMPRODUCT(($B$35-D5) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I5</f>
-        <v>71700.343074295219</v>
+        <v>76138.330847275065</v>
       </c>
     </row>
     <row r="6" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>30</v>
       </c>
-      <c r="B6">
-        <v>216.430172350898</v>
-      </c>
-      <c r="C6">
-        <v>95.186186205874094</v>
-      </c>
-      <c r="D6">
-        <v>22.506067658953899</v>
+      <c r="B6" s="1">
+        <v>88.322656699999996</v>
+      </c>
+      <c r="C6" s="1">
+        <v>4.9276398800000001</v>
+      </c>
+      <c r="D6" s="1">
+        <v>-46.978507</v>
       </c>
       <c r="F6">
         <v>30</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="7">
         <f t="shared" si="3"/>
-        <v>25000</v>
-      </c>
-      <c r="H6">
+        <v>23722</v>
+      </c>
+      <c r="H6" s="7">
         <f t="shared" si="3"/>
-        <v>26200</v>
-      </c>
-      <c r="I6">
+        <v>25538</v>
+      </c>
+      <c r="I6" s="7">
         <f t="shared" si="3"/>
-        <v>27280</v>
+        <v>27172.400000000001</v>
       </c>
       <c r="K6">
         <v>30</v>
       </c>
-      <c r="L6" s="2">
+      <c r="L6" s="6">
         <f t="shared" si="4"/>
-        <v>6.6102793105964078E-2</v>
-      </c>
-      <c r="M6" s="2">
+        <v>7.5064385098221068E-2</v>
+      </c>
+      <c r="M6" s="6">
         <f t="shared" si="1"/>
-        <v>6.7702817320386494E-2</v>
-      </c>
-      <c r="N6" s="2">
+        <v>7.2992104319837103E-2</v>
+      </c>
+      <c r="N6" s="6">
         <f t="shared" si="1"/>
-        <v>6.7686727725111653E-2</v>
+        <v>7.0511935162149819E-2</v>
       </c>
       <c r="P6">
         <v>30</v>
       </c>
       <c r="Q6" s="4">
         <f t="shared" si="5"/>
-        <v>11.128198885807679</v>
+        <v>10.117283613021128</v>
       </c>
       <c r="R6" s="4">
         <f t="shared" si="2"/>
-        <v>10.932678605758907</v>
+        <v>10.33388820420411</v>
       </c>
       <c r="S6" s="4">
         <f t="shared" si="2"/>
-        <v>10.934609412194733</v>
+        <v>10.606024337925726</v>
       </c>
       <c r="U6">
         <v>30</v>
       </c>
-      <c r="V6" s="6" cm="1">
+      <c r="V6" s="5" cm="1">
         <f t="array" ref="V6">SUMPRODUCT(($B$35-B6) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G6</f>
-        <v>13173.457698006721</v>
-      </c>
-      <c r="W6" s="6" cm="1">
+        <v>17410.671128916983</v>
+      </c>
+      <c r="W6" s="5" cm="1">
         <f t="array" ref="W6">SUMPRODUCT(($B$35-C6) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H6</f>
-        <v>14774.127357351084</v>
-      </c>
-      <c r="X6" s="6" cm="1">
+        <v>17521.050331502054</v>
+      </c>
+      <c r="X6" s="5" cm="1">
         <f t="array" ref="X6">SUMPRODUCT(($B$35-D6) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I6</f>
-        <v>15372.998279727668</v>
+        <v>17085.653888894209</v>
       </c>
       <c r="Z6">
         <v>30</v>
       </c>
-      <c r="AA6" s="6" cm="1">
+      <c r="AA6" s="5" cm="1">
         <f t="array" ref="AA6">SUMPRODUCT(($B$35-B6) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G6</f>
-        <v>64400.807498104317</v>
-      </c>
-      <c r="AB6" s="6" cm="1">
+        <v>72609.174466051976</v>
+      </c>
+      <c r="AB6" s="5" cm="1">
         <f t="array" ref="AB6">SUMPRODUCT(($B$35-C6) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H6</f>
-        <v>69759.870893975327</v>
-      </c>
-      <c r="AC6" s="6" cm="1">
+        <v>75304.68237348611</v>
+      </c>
+      <c r="AC6" s="5" cm="1">
         <f t="array" ref="AC6">SUMPRODUCT(($B$35-D6) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I6</f>
-        <v>72611.723683757882</v>
+        <v>76478.303775999899</v>
       </c>
     </row>
     <row r="7" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>40</v>
       </c>
-      <c r="B7">
-        <v>212.32790632726099</v>
-      </c>
-      <c r="C7">
-        <v>90.071446030303505</v>
-      </c>
-      <c r="D7">
-        <v>25.748762016457299</v>
+      <c r="B7" s="1">
+        <v>80.195430400000006</v>
+      </c>
+      <c r="C7" s="1">
+        <v>6.2776308800000002</v>
+      </c>
+      <c r="D7" s="1">
+        <v>-41.859730999999996</v>
       </c>
       <c r="F7">
         <v>40</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="7">
         <f t="shared" si="3"/>
-        <v>25000</v>
-      </c>
-      <c r="H7">
+        <v>23722</v>
+      </c>
+      <c r="H7" s="7">
         <f t="shared" si="3"/>
-        <v>26200</v>
-      </c>
-      <c r="I7">
+        <v>25538</v>
+      </c>
+      <c r="I7" s="7">
         <f t="shared" si="3"/>
-        <v>27280</v>
+        <v>27172.400000000001</v>
       </c>
       <c r="K7">
         <v>40</v>
       </c>
-      <c r="L7" s="2">
+      <c r="L7" s="6">
         <f t="shared" si="4"/>
-        <v>6.6266883746909561E-2</v>
-      </c>
-      <c r="M7" s="2">
+        <v>7.5406988011128911E-2</v>
+      </c>
+      <c r="M7" s="6">
         <f t="shared" si="1"/>
-        <v>6.7898036411057114E-2</v>
-      </c>
-      <c r="N7" s="2">
+        <v>7.2939242271125374E-2</v>
+      </c>
+      <c r="N7" s="6">
         <f t="shared" si="1"/>
-        <v>6.7567860629895268E-2</v>
+        <v>7.0323553716270915E-2</v>
       </c>
       <c r="P7">
         <v>40</v>
       </c>
       <c r="Q7" s="4">
         <f t="shared" si="5"/>
-        <v>11.107815261271979</v>
+        <v>10.082368936338812</v>
       </c>
       <c r="R7" s="4">
         <f t="shared" si="2"/>
-        <v>10.909307614576283</v>
+        <v>10.3395385092795</v>
       </c>
       <c r="S7" s="4">
         <f t="shared" si="2"/>
-        <v>10.948895718544703</v>
+        <v>10.627299364420749</v>
       </c>
       <c r="U7">
         <v>40</v>
       </c>
-      <c r="V7" s="6" cm="1">
+      <c r="V7" s="5" cm="1">
         <f t="array" ref="V7">SUMPRODUCT(($B$35-B7) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G7</f>
-        <v>13268.217795824821</v>
-      </c>
-      <c r="W7" s="6" cm="1">
+        <v>17598.405604141262</v>
+      </c>
+      <c r="W7" s="5" cm="1">
         <f t="array" ref="W7">SUMPRODUCT(($B$35-C7) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H7</f>
-        <v>14892.275053419202</v>
-      </c>
-      <c r="X7" s="6" cm="1">
+        <v>17489.866278962203</v>
+      </c>
+      <c r="X7" s="5" cm="1">
         <f t="array" ref="X7">SUMPRODUCT(($B$35-D7) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I7</f>
-        <v>15298.093816501554</v>
+        <v>16967.412967492688</v>
       </c>
       <c r="Z7">
         <v>40</v>
       </c>
-      <c r="AA7" s="6" cm="1">
+      <c r="AA7" s="5" cm="1">
         <f t="array" ref="AA7">SUMPRODUCT(($B$35-B7) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G7</f>
-        <v>64622.732096356776</v>
-      </c>
-      <c r="AB7" s="6" cm="1">
+        <v>73048.84157226645</v>
+      </c>
+      <c r="AB7" s="5" cm="1">
         <f t="array" ref="AB7">SUMPRODUCT(($B$35-C7) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H7</f>
-        <v>70036.568370952431</v>
-      </c>
-      <c r="AC7" s="6" cm="1">
+        <v>75231.650490962347</v>
+      </c>
+      <c r="AC7" s="5" cm="1">
         <f t="array" ref="AC7">SUMPRODUCT(($B$35-D7) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I7</f>
-        <v>72436.300237692209</v>
+        <v>76201.387968785333</v>
       </c>
     </row>
     <row r="8" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>50</v>
       </c>
-      <c r="B8">
-        <v>227.67570194637699</v>
-      </c>
-      <c r="C8">
-        <v>105.20930495038</v>
-      </c>
-      <c r="D8">
-        <v>40.666234150020301</v>
+      <c r="B8" s="1">
+        <v>85.289489900000007</v>
+      </c>
+      <c r="C8" s="1">
+        <v>16.259692399999999</v>
+      </c>
+      <c r="D8" s="1">
+        <v>-29.748246999999999</v>
       </c>
       <c r="F8">
         <v>50</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="7">
         <f t="shared" si="3"/>
-        <v>25000</v>
-      </c>
-      <c r="H8">
+        <v>23722</v>
+      </c>
+      <c r="H8" s="7">
         <f t="shared" si="3"/>
-        <v>26200</v>
-      </c>
-      <c r="I8">
+        <v>25538</v>
+      </c>
+      <c r="I8" s="7">
         <f t="shared" si="3"/>
-        <v>27280</v>
+        <v>27172.400000000001</v>
       </c>
       <c r="K8">
         <v>50</v>
       </c>
-      <c r="L8" s="2">
+      <c r="L8" s="6">
         <f t="shared" si="4"/>
-        <v>6.565297192214492E-2</v>
-      </c>
-      <c r="M8" s="2">
+        <v>7.5192248128319705E-2</v>
+      </c>
+      <c r="M8" s="6">
         <f t="shared" si="1"/>
-        <v>6.732025553624503E-2</v>
-      </c>
-      <c r="N8" s="2">
+        <v>7.2548371352494326E-2</v>
+      </c>
+      <c r="N8" s="6">
         <f t="shared" si="1"/>
-        <v>6.7021032472506584E-2</v>
+        <v>6.9877826286967648E-2</v>
       </c>
       <c r="P8">
         <v>50</v>
       </c>
       <c r="Q8" s="4">
         <f t="shared" si="5"/>
-        <v>11.184475147099118</v>
+        <v>10.104224054365075</v>
       </c>
       <c r="R8" s="4">
         <f t="shared" si="2"/>
-        <v>10.978778828001003</v>
+        <v>10.38151600347854</v>
       </c>
       <c r="S8" s="4">
         <f t="shared" si="2"/>
-        <v>11.015117243049076</v>
+        <v>10.677990105102017</v>
       </c>
       <c r="U8">
         <v>50</v>
       </c>
-      <c r="V8" s="6" cm="1">
+      <c r="V8" s="5" cm="1">
         <f t="array" ref="V8">SUMPRODUCT(($B$35-B8) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G8</f>
-        <v>12913.692124944435</v>
-      </c>
-      <c r="W8" s="6" cm="1">
+        <v>17480.735620349406</v>
+      </c>
+      <c r="W8" s="5" cm="1">
         <f t="array" ref="W8">SUMPRODUCT(($B$35-C8) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H8</f>
-        <v>14542.598805277856</v>
-      </c>
-      <c r="X8" s="6" cm="1">
+        <v>17259.286126282852</v>
+      </c>
+      <c r="X8" s="5" cm="1">
         <f t="array" ref="X8">SUMPRODUCT(($B$35-D8) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I8</f>
-        <v>14953.508382395063</v>
+        <v>16687.644322078289</v>
       </c>
       <c r="Z8">
         <v>50</v>
       </c>
-      <c r="AA8" s="6" cm="1">
+      <c r="AA8" s="5" cm="1">
         <f t="array" ref="AA8">SUMPRODUCT(($B$35-B8) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G8</f>
-        <v>63792.446259892735</v>
-      </c>
-      <c r="AB8" s="6" cm="1">
+        <v>72773.262879539601</v>
+      </c>
+      <c r="AB8" s="5" cm="1">
         <f t="array" ref="AB8">SUMPRODUCT(($B$35-C8) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H8</f>
-        <v>69217.639700826301</v>
-      </c>
-      <c r="AC8" s="6" cm="1">
+        <v>74691.640413655507</v>
+      </c>
+      <c r="AC8" s="5" cm="1">
         <f t="array" ref="AC8">SUMPRODUCT(($B$35-D8) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I8</f>
-        <v>71629.294063273439</v>
+        <v>75546.18028467751</v>
       </c>
     </row>
     <row r="9" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>60</v>
       </c>
-      <c r="B9">
-        <v>264.44575797169398</v>
-      </c>
-      <c r="C9">
-        <v>133.46562806209101</v>
-      </c>
-      <c r="D9">
-        <v>67.899706915627405</v>
+      <c r="B9" s="1">
+        <v>103.284909</v>
+      </c>
+      <c r="C9" s="1">
+        <v>32.507283600000001</v>
+      </c>
+      <c r="D9" s="1">
+        <v>-10.177547000000001</v>
       </c>
       <c r="F9">
         <v>60</v>
       </c>
-      <c r="G9">
+      <c r="G9" s="7">
         <f t="shared" si="3"/>
-        <v>25000</v>
-      </c>
-      <c r="H9">
+        <v>23722</v>
+      </c>
+      <c r="H9" s="7">
         <f t="shared" si="3"/>
-        <v>26200</v>
-      </c>
-      <c r="I9">
+        <v>25538</v>
+      </c>
+      <c r="I9" s="7">
         <f t="shared" si="3"/>
-        <v>27280</v>
+        <v>27172.400000000001</v>
       </c>
       <c r="K9">
         <v>60</v>
       </c>
-      <c r="L9" s="2">
+      <c r="L9" s="6">
         <f t="shared" si="4"/>
-        <v>6.4182169681132231E-2</v>
-      </c>
-      <c r="M9" s="2">
+        <v>7.4433651926481742E-2</v>
+      </c>
+      <c r="M9" s="6">
         <f t="shared" si="1"/>
-        <v>6.6241769921294227E-2</v>
-      </c>
-      <c r="N9" s="2">
+        <v>7.1912158994439659E-2</v>
+      </c>
+      <c r="N9" s="6">
         <f t="shared" si="1"/>
-        <v>6.6022738016289315E-2</v>
+        <v>6.9157584423900714E-2</v>
       </c>
       <c r="P9">
         <v>60</v>
       </c>
       <c r="Q9" s="4">
         <f t="shared" si="5"/>
-        <v>11.372666638892303</v>
+        <v>10.18221607041432</v>
       </c>
       <c r="R9" s="4">
         <f t="shared" si="2"/>
-        <v>11.110929940626836</v>
+        <v>10.4505974674559</v>
       </c>
       <c r="S9" s="4">
         <f t="shared" si="2"/>
-        <v>11.138171561801459</v>
+        <v>10.760962673877161</v>
       </c>
       <c r="U9">
         <v>60</v>
       </c>
-      <c r="V9" s="6" cm="1">
+      <c r="V9" s="5" cm="1">
         <f t="array" ref="V9">SUMPRODUCT(($B$35-B9) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G9</f>
-        <v>12064.323974351631</v>
-      </c>
-      <c r="W9" s="6" cm="1">
+        <v>17065.051297497528</v>
+      </c>
+      <c r="W9" s="5" cm="1">
         <f t="array" ref="W9">SUMPRODUCT(($B$35-C9) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H9</f>
-        <v>13889.893220945261</v>
-      </c>
-      <c r="X9" s="6" cm="1">
+        <v>16883.975670415442</v>
+      </c>
+      <c r="X9" s="5" cm="1">
         <f t="array" ref="X9">SUMPRODUCT(($B$35-D9) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I9</f>
-        <v>14324.430080713486</v>
+        <v>16235.571873416229</v>
       </c>
       <c r="Z9">
         <v>60</v>
       </c>
-      <c r="AA9" s="6" cm="1">
+      <c r="AA9" s="5" cm="1">
         <f t="array" ref="AA9">SUMPRODUCT(($B$35-B9) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G9</f>
-        <v>61803.257878612494</v>
-      </c>
-      <c r="AB9" s="6" cm="1">
+        <v>71799.745771887043</v>
+      </c>
+      <c r="AB9" s="5" cm="1">
         <f t="array" ref="AB9">SUMPRODUCT(($B$35-C9) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H9</f>
-        <v>67689.027680414496</v>
-      </c>
-      <c r="AC9" s="6" cm="1">
+        <v>73812.677389596531</v>
+      </c>
+      <c r="AC9" s="5" cm="1">
         <f t="array" ref="AC9">SUMPRODUCT(($B$35-D9) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I9</f>
-        <v>70156.016253471942</v>
+        <v>74487.443549908436</v>
       </c>
     </row>
     <row r="10" spans="1:29" ht="19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>70</v>
       </c>
-      <c r="B10">
-        <v>330.23111627159801</v>
-      </c>
-      <c r="C10">
-        <v>186.560287706151</v>
-      </c>
-      <c r="D10">
-        <v>110.197744440671</v>
+      <c r="B10" s="1">
+        <v>137.07569599999999</v>
+      </c>
+      <c r="C10" s="1">
+        <v>60.526115500000003</v>
+      </c>
+      <c r="D10" s="1">
+        <v>14.130844700000001</v>
       </c>
       <c r="F10">
         <v>70</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="7">
         <f t="shared" si="3"/>
-        <v>25000</v>
-      </c>
-      <c r="H10">
+        <v>23722</v>
+      </c>
+      <c r="H10" s="7">
         <f t="shared" si="3"/>
-        <v>26200</v>
-      </c>
-      <c r="I10">
+        <v>25538</v>
+      </c>
+      <c r="I10" s="7">
         <f t="shared" si="3"/>
-        <v>27280</v>
+        <v>27172.400000000001</v>
       </c>
       <c r="K10">
         <v>70</v>
       </c>
-      <c r="L10" s="2">
+      <c r="L10" s="6">
         <f t="shared" si="4"/>
-        <v>6.155075534913608E-2</v>
-      </c>
-      <c r="M10" s="2">
+        <v>7.3009202596745648E-2</v>
+      </c>
+      <c r="M10" s="6">
         <f t="shared" si="1"/>
-        <v>6.4215256194421713E-2</v>
-      </c>
-      <c r="N10" s="2">
+        <v>7.0815016230715011E-2</v>
+      </c>
+      <c r="N10" s="6">
         <f t="shared" si="1"/>
-        <v>6.4472223444256932E-2</v>
+        <v>6.8262985798089232E-2</v>
       </c>
       <c r="P10">
         <v>70</v>
       </c>
       <c r="Q10" s="4">
         <f t="shared" si="5"/>
-        <v>11.726261920498374</v>
+        <v>10.332061967930757</v>
       </c>
       <c r="R10" s="4">
         <f t="shared" si="2"/>
-        <v>11.368361115317519</v>
+        <v>10.571979221347535</v>
       </c>
       <c r="S10" s="4">
         <f t="shared" si="2"/>
-        <v>11.335036676572404</v>
+        <v>10.865892573391662</v>
       </c>
       <c r="U10">
         <v>70</v>
       </c>
-      <c r="V10" s="6" cm="1">
+      <c r="V10" s="5" cm="1">
         <f t="array" ref="V10">SUMPRODUCT(($B$35-B10) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G10</f>
-        <v>10544.718236552326</v>
-      </c>
-      <c r="W10" s="6" cm="1">
+        <v>16284.50262926858</v>
+      </c>
+      <c r="W10" s="5" cm="1">
         <f t="array" ref="W10">SUMPRODUCT(($B$35-C10) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H10</f>
-        <v>12663.435669801504</v>
-      </c>
-      <c r="X10" s="6" cm="1">
+        <v>16236.756002969516</v>
+      </c>
+      <c r="X10" s="5" cm="1">
         <f t="array" ref="X10">SUMPRODUCT(($B$35-D10) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I10</f>
-        <v>13347.36858584889</v>
+        <v>15674.061341914778</v>
       </c>
       <c r="Z10">
         <v>70</v>
       </c>
-      <c r="AA10" s="6" cm="1">
+      <c r="AA10" s="5" cm="1">
         <f t="array" ref="AA10">SUMPRODUCT(($B$35-B10) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G10</f>
-        <v>58244.39818314655</v>
-      </c>
-      <c r="AB10" s="6" cm="1">
+        <v>69971.73003950862</v>
+      </c>
+      <c r="AB10" s="5" cm="1">
         <f t="array" ref="AB10">SUMPRODUCT(($B$35-C10) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H10</f>
-        <v>64816.710053286763</v>
-      </c>
-      <c r="AC10" s="6" cm="1">
+        <v>72296.913180965726</v>
+      </c>
+      <c r="AC10" s="5" cm="1">
         <f t="array" ref="AC10">SUMPRODUCT(($B$35-D10) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I10</f>
-        <v>67867.774844814849</v>
+        <v>73172.406925978488</v>
       </c>
     </row>
     <row r="11" spans="1:29" x14ac:dyDescent="0.2">
@@ -1850,88 +1855,88 @@
         <v>0</v>
       </c>
       <c r="B13">
-        <v>402.39581604809899</v>
+        <v>241.89738568160499</v>
       </c>
       <c r="C13">
-        <v>290.29298109553798</v>
+        <v>156.54610689144201</v>
       </c>
       <c r="D13">
-        <v>214.88456485730799</v>
+        <v>93.391055442071007</v>
       </c>
       <c r="F13">
         <v>0</v>
       </c>
-      <c r="G13">
+      <c r="G13" s="7">
         <f>$B$11*$B$32+$B$34*G$12</f>
-        <v>15200</v>
-      </c>
-      <c r="H13">
+        <v>15947</v>
+      </c>
+      <c r="H13" s="7">
         <f t="shared" ref="H13:I13" si="6">$B$11*$B$32+$B$34*H$12</f>
-        <v>16400</v>
-      </c>
-      <c r="I13">
+        <v>17763</v>
+      </c>
+      <c r="I13" s="7">
         <f t="shared" si="6"/>
-        <v>17480</v>
+        <v>19397.400000000001</v>
       </c>
       <c r="K13">
         <v>0</v>
       </c>
-      <c r="L13" s="2">
+      <c r="L13" s="6">
         <f>($B$35-B13)/G13</f>
-        <v>9.6487117365256642E-2</v>
-      </c>
-      <c r="M13" s="2">
+        <v>0.10203189404392017</v>
+      </c>
+      <c r="M13" s="6">
         <f t="shared" ref="M13:M20" si="7">($B$35-C13)/H13</f>
-        <v>9.626262310393062E-2</v>
-      </c>
-      <c r="N13" s="2">
+        <v>9.6405668699462821E-2</v>
+      </c>
+      <c r="N13" s="6">
         <f t="shared" ref="N13:N20" si="8">($B$35-D13)/I13</f>
-        <v>9.4629029470405718E-2</v>
+        <v>9.1538502302263638E-2</v>
       </c>
       <c r="P13">
         <v>0</v>
       </c>
       <c r="Q13" s="4">
         <f>LN(1+(G13*$B$36/($B$35-B13)))/LN(1+$B$36)</f>
-        <v>8.3236428524917407</v>
+        <v>7.9601650868476694</v>
       </c>
       <c r="R13" s="4">
         <f t="shared" ref="R13:R20" si="9">LN(1+(H13*$B$36/($B$35-C13)))/LN(1+$B$36)</f>
-        <v>8.3390729437913578</v>
+        <v>8.329234307445299</v>
       </c>
       <c r="S13" s="4">
         <f t="shared" ref="S13:S20" si="10">LN(1+(I13*$B$36/($B$35-D13)))/LN(1+$B$36)</f>
-        <v>8.4531345702715015</v>
+        <v>8.6778653056310002</v>
       </c>
       <c r="U13">
         <v>0</v>
       </c>
-      <c r="V13" s="6" cm="1">
+      <c r="V13" s="5" cm="1">
         <f t="array" ref="V13">SUMPRODUCT(($B$35-B13) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G13</f>
-        <v>18677.753205412628</v>
-      </c>
-      <c r="W13" s="6" cm="1">
+        <v>21638.179021668519</v>
+      </c>
+      <c r="W13" s="5" cm="1">
         <f t="array" ref="W13">SUMPRODUCT(($B$35-C13) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H13</f>
-        <v>20067.267279971224</v>
-      </c>
-      <c r="X13" s="6" cm="1">
+        <v>21793.74680407322</v>
+      </c>
+      <c r="X13" s="5" cm="1">
         <f t="array" ref="X13">SUMPRODUCT(($B$35-D13) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I13</f>
-        <v>20729.160384384704</v>
+        <v>21618.193894575663</v>
       </c>
       <c r="Z13">
         <v>0</v>
       </c>
-      <c r="AA13" s="6" cm="1">
+      <c r="AA13" s="5" cm="1">
         <f t="array" ref="AA13">SUMPRODUCT(($B$35-B13) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G13</f>
-        <v>64140.428544504859</v>
-      </c>
-      <c r="AB13" s="6" cm="1">
+        <v>72076.080882018985</v>
+      </c>
+      <c r="AB13" s="5" cm="1">
         <f t="array" ref="AB13">SUMPRODUCT(($B$35-C13) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H13</f>
-        <v>69004.973473201011</v>
-      </c>
-      <c r="AC13" s="6" cm="1">
+        <v>74877.418750090379</v>
+      </c>
+      <c r="AC13" s="5" cm="1">
         <f t="array" ref="AC13">SUMPRODUCT(($B$35-D13) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I13</f>
-        <v>72004.421851755338</v>
+        <v>76659.583970326843</v>
       </c>
     </row>
     <row r="14" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -1939,88 +1944,88 @@
         <v>10</v>
       </c>
       <c r="B14">
-        <v>344.47030026312399</v>
+        <v>192.85892812091399</v>
       </c>
       <c r="C14">
-        <v>240.18294573265101</v>
+        <v>115.109022116007</v>
       </c>
       <c r="D14">
-        <v>175.052667632083</v>
+        <v>60.706040317261802</v>
       </c>
       <c r="F14">
         <v>10</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="7">
         <f t="shared" ref="G14:I20" si="11">$B$11*$B$32+$B$34*G$12</f>
-        <v>15200</v>
-      </c>
-      <c r="H14">
+        <v>15947</v>
+      </c>
+      <c r="H14" s="7">
         <f t="shared" si="11"/>
-        <v>16400</v>
-      </c>
-      <c r="I14">
+        <v>17763</v>
+      </c>
+      <c r="I14" s="7">
         <f t="shared" si="11"/>
-        <v>17480</v>
+        <v>19397.400000000001</v>
       </c>
       <c r="K14">
         <v>10</v>
       </c>
-      <c r="L14" s="2">
+      <c r="L14" s="6">
         <f t="shared" ref="L14:L20" si="12">($B$35-B14)/G14</f>
-        <v>0.10029800656163658</v>
-      </c>
-      <c r="M14" s="2">
+        <v>0.10510698387653389</v>
+      </c>
+      <c r="M14" s="6">
         <f t="shared" si="7"/>
-        <v>9.9318113065082259E-2</v>
-      </c>
-      <c r="N14" s="2">
+        <v>9.8738443837414452E-2</v>
+      </c>
+      <c r="N14" s="6">
         <f t="shared" si="8"/>
-        <v>9.6907742126311036E-2</v>
+        <v>9.3223522723805158E-2</v>
       </c>
       <c r="P14">
         <v>10</v>
       </c>
       <c r="Q14" s="4">
         <f t="shared" ref="Q14:Q20" si="13">LN(1+(G14*$B$36/($B$35-B14)))/LN(1+$B$36)</f>
-        <v>8.0703069420209861</v>
+        <v>7.7721641967317083</v>
       </c>
       <c r="R14" s="4">
         <f t="shared" si="9"/>
-        <v>8.1339359605549717</v>
+        <v>8.1720597581859078</v>
       </c>
       <c r="S14" s="4">
         <f t="shared" si="10"/>
-        <v>8.294888255919517</v>
+        <v>8.5538479799807696</v>
       </c>
       <c r="U14">
         <v>10</v>
       </c>
-      <c r="V14" s="6" cm="1">
+      <c r="V14" s="5" cm="1">
         <f t="array" ref="V14">SUMPRODUCT(($B$35-B14) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G14</f>
-        <v>20015.800886943012</v>
-      </c>
-      <c r="W14" s="6" cm="1">
+        <v>22770.940526779341</v>
+      </c>
+      <c r="W14" s="5" cm="1">
         <f t="array" ref="W14">SUMPRODUCT(($B$35-C14) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H14</f>
-        <v>21224.781645274612</v>
-      </c>
-      <c r="X14" s="6" cm="1">
+        <v>22750.920762074144</v>
+      </c>
+      <c r="X14" s="5" cm="1">
         <f t="array" ref="X14">SUMPRODUCT(($B$35-D14) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I14</f>
-        <v>21649.255389339218</v>
+        <v>22373.199838258268</v>
       </c>
       <c r="Z14">
         <v>10</v>
       </c>
-      <c r="AA14" s="6" cm="1">
+      <c r="AA14" s="5" cm="1">
         <f t="array" ref="AA14">SUMPRODUCT(($B$35-B14) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G14</f>
-        <v>67274.086075507861</v>
-      </c>
-      <c r="AB14" s="6" cm="1">
+        <v>74728.965880303091</v>
+      </c>
+      <c r="AB14" s="5" cm="1">
         <f t="array" ref="AB14">SUMPRODUCT(($B$35-C14) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H14</f>
-        <v>71715.828742520331</v>
-      </c>
-      <c r="AC14" s="6" cm="1">
+        <v>77119.084292635831</v>
+      </c>
+      <c r="AC14" s="5" cm="1">
         <f t="array" ref="AC14">SUMPRODUCT(($B$35-D14) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I14</f>
-        <v>74159.249875683599</v>
+        <v>78427.779598951194</v>
       </c>
     </row>
     <row r="15" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -2028,88 +2033,88 @@
         <v>20</v>
       </c>
       <c r="B15">
-        <v>313.06513116860702</v>
+        <v>166.12677657953199</v>
       </c>
       <c r="C15">
-        <v>220.165993309546</v>
+        <v>99.152232800197098</v>
       </c>
       <c r="D15">
-        <v>161.811646215439</v>
+        <v>48.205357316342699</v>
       </c>
       <c r="F15">
         <v>20</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="7">
         <f t="shared" si="11"/>
-        <v>15200</v>
-      </c>
-      <c r="H15">
+        <v>15947</v>
+      </c>
+      <c r="H15" s="7">
         <f t="shared" si="11"/>
-        <v>16400</v>
-      </c>
-      <c r="I15">
+        <v>17763</v>
+      </c>
+      <c r="I15" s="7">
         <f t="shared" si="11"/>
-        <v>17480</v>
+        <v>19397.400000000001</v>
       </c>
       <c r="K15">
         <v>20</v>
       </c>
-      <c r="L15" s="2">
+      <c r="L15" s="6">
         <f t="shared" si="12"/>
-        <v>0.10236413610732849</v>
-      </c>
-      <c r="M15" s="2">
+        <v>0.10678329613221722</v>
+      </c>
+      <c r="M15" s="6">
         <f t="shared" si="7"/>
-        <v>0.10053865894453988</v>
-      </c>
-      <c r="N15" s="2">
+        <v>9.9636759961707094E-2</v>
+      </c>
+      <c r="N15" s="6">
         <f t="shared" si="8"/>
-        <v>9.7665237630695706E-2</v>
+        <v>9.3867974196730333E-2</v>
       </c>
       <c r="P15">
         <v>20</v>
       </c>
       <c r="Q15" s="4">
         <f t="shared" si="13"/>
-        <v>7.9394082731689934</v>
+        <v>7.6734316318961575</v>
       </c>
       <c r="R15" s="4">
         <f t="shared" si="9"/>
-        <v>8.0548349311527172</v>
+        <v>8.1131329655551809</v>
       </c>
       <c r="S15" s="4">
         <f t="shared" si="10"/>
-        <v>8.2436118068994144</v>
+        <v>8.5073668241639435</v>
       </c>
       <c r="U15">
         <v>20</v>
       </c>
-      <c r="V15" s="6" cm="1">
+      <c r="V15" s="5" cm="1">
         <f t="array" ref="V15">SUMPRODUCT(($B$35-B15) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G15</f>
-        <v>20741.243088458781</v>
-      </c>
-      <c r="W15" s="6" cm="1">
+        <v>23388.438582818118</v>
+      </c>
+      <c r="W15" s="5" cm="1">
         <f t="array" ref="W15">SUMPRODUCT(($B$35-C15) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H15</f>
-        <v>21687.162280441735</v>
-      </c>
-      <c r="X15" s="6" cm="1">
+        <v>23119.513853725592</v>
+      </c>
+      <c r="X15" s="5" cm="1">
         <f t="array" ref="X15">SUMPRODUCT(($B$35-D15) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I15</f>
-        <v>21955.11573028814</v>
+        <v>22661.958767380558</v>
       </c>
       <c r="Z15">
         <v>20</v>
       </c>
-      <c r="AA15" s="6" cm="1">
+      <c r="AA15" s="5" cm="1">
         <f t="array" ref="AA15">SUMPRODUCT(($B$35-B15) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G15</f>
-        <v>68973.044527786013</v>
-      </c>
-      <c r="AB15" s="6" cm="1">
+        <v>76175.123188742538</v>
+      </c>
+      <c r="AB15" s="5" cm="1">
         <f t="array" ref="AB15">SUMPRODUCT(($B$35-C15) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H15</f>
-        <v>72798.706863817264</v>
-      </c>
-      <c r="AC15" s="6" cm="1">
+        <v>77982.315501413192</v>
+      </c>
+      <c r="AC15" s="5" cm="1">
         <f t="array" ref="AC15">SUMPRODUCT(($B$35-D15) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I15</f>
-        <v>74875.563333028811</v>
+        <v>79104.04219062021</v>
       </c>
     </row>
     <row r="16" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -2117,88 +2122,88 @@
         <v>30</v>
       </c>
       <c r="B16">
-        <v>303.21734076172498</v>
+        <v>157.71876924567499</v>
       </c>
       <c r="C16">
-        <v>220.10625080158999</v>
+        <v>95.412080648464098</v>
       </c>
       <c r="D16">
-        <v>160.05753879151899</v>
+        <v>47.443542770563901</v>
       </c>
       <c r="F16">
         <v>30</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="7">
         <f t="shared" si="11"/>
-        <v>15200</v>
-      </c>
-      <c r="H16">
+        <v>15947</v>
+      </c>
+      <c r="H16" s="7">
         <f t="shared" si="11"/>
-        <v>16400</v>
-      </c>
-      <c r="I16">
+        <v>17763</v>
+      </c>
+      <c r="I16" s="7">
         <f t="shared" si="11"/>
-        <v>17480</v>
+        <v>19397.400000000001</v>
       </c>
       <c r="K16">
         <v>30</v>
       </c>
-      <c r="L16" s="2">
+      <c r="L16" s="6">
         <f t="shared" si="12"/>
-        <v>0.10301201705514967</v>
-      </c>
-      <c r="M16" s="2">
+        <v>0.10731054309615132</v>
+      </c>
+      <c r="M16" s="6">
         <f t="shared" si="7"/>
-        <v>0.10054230178039085</v>
-      </c>
-      <c r="N16" s="2">
+        <v>9.9847318547066147E-2</v>
+      </c>
+      <c r="N16" s="6">
         <f t="shared" si="8"/>
-        <v>9.7765587025656811E-2</v>
+        <v>9.3907248251282952E-2</v>
       </c>
       <c r="P16">
         <v>30</v>
       </c>
       <c r="Q16" s="4">
         <f t="shared" si="13"/>
-        <v>7.8992469904828431</v>
+        <v>7.6429022267578537</v>
       </c>
       <c r="R16" s="4">
         <f t="shared" si="9"/>
-        <v>8.054601189993015</v>
+        <v>8.0994458943817822</v>
       </c>
       <c r="S16" s="4">
         <f t="shared" si="10"/>
-        <v>8.2368673419805738</v>
+        <v>8.5045508244226244</v>
       </c>
       <c r="U16">
         <v>30</v>
       </c>
-      <c r="V16" s="6" cm="1">
+      <c r="V16" s="5" cm="1">
         <f t="array" ref="V16">SUMPRODUCT(($B$35-B16) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G16</f>
-        <v>20968.721651982312</v>
-      </c>
-      <c r="W16" s="6" cm="1">
+        <v>23582.658946105345</v>
+      </c>
+      <c r="W16" s="5" cm="1">
         <f t="array" ref="W16">SUMPRODUCT(($B$35-C16) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H16</f>
-        <v>21688.542299647022</v>
-      </c>
-      <c r="X16" s="6" cm="1">
+        <v>23205.909319478102</v>
+      </c>
+      <c r="X16" s="5" cm="1">
         <f t="array" ref="X16">SUMPRODUCT(($B$35-D16) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I16</f>
-        <v>21995.634650835076</v>
+        <v>22679.556266046253</v>
       </c>
       <c r="Z16">
         <v>30</v>
       </c>
-      <c r="AA16" s="6" cm="1">
+      <c r="AA16" s="5" cm="1">
         <f t="array" ref="AA16">SUMPRODUCT(($B$35-B16) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G16</f>
-        <v>69505.790799512266</v>
-      </c>
-      <c r="AB16" s="6" cm="1">
+        <v>76629.980001762131</v>
+      </c>
+      <c r="AB16" s="5" cm="1">
         <f t="array" ref="AB16">SUMPRODUCT(($B$35-C16) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H16</f>
-        <v>72801.938817084185</v>
-      </c>
-      <c r="AC16" s="6" cm="1">
+        <v>78184.650444806408</v>
+      </c>
+      <c r="AC16" s="5" cm="1">
         <f t="array" ref="AC16">SUMPRODUCT(($B$35-D16) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I16</f>
-        <v>74970.457126630237</v>
+        <v>79145.254873084166</v>
       </c>
     </row>
     <row r="17" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -2206,88 +2211,88 @@
         <v>40</v>
       </c>
       <c r="B17">
-        <v>312.24957418687501</v>
+        <v>161.39266757354099</v>
       </c>
       <c r="C17">
-        <v>228.45362120177001</v>
+        <v>101.25617285685701</v>
       </c>
       <c r="D17">
-        <v>170.79751470113399</v>
+        <v>55.748770128589797</v>
       </c>
       <c r="F17">
         <v>40</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="7">
         <f t="shared" si="11"/>
-        <v>15200</v>
-      </c>
-      <c r="H17">
+        <v>15947</v>
+      </c>
+      <c r="H17" s="7">
         <f t="shared" si="11"/>
-        <v>16400</v>
-      </c>
-      <c r="I17">
+        <v>17763</v>
+      </c>
+      <c r="I17" s="7">
         <f t="shared" si="11"/>
-        <v>17480</v>
+        <v>19397.400000000001</v>
       </c>
       <c r="K17">
         <v>40</v>
       </c>
-      <c r="L17" s="2">
+      <c r="L17" s="6">
         <f t="shared" si="12"/>
-        <v>0.10241779117191613</v>
-      </c>
-      <c r="M17" s="2">
+        <v>0.10708016131099636</v>
+      </c>
+      <c r="M17" s="6">
         <f t="shared" si="7"/>
-        <v>0.10003331578037988</v>
-      </c>
-      <c r="N17" s="2">
+        <v>9.9518314876042499E-2</v>
+      </c>
+      <c r="N17" s="6">
         <f t="shared" si="8"/>
-        <v>9.7151171927852747E-2</v>
+        <v>9.3479086365771194E-2</v>
       </c>
       <c r="P17">
         <v>40</v>
       </c>
       <c r="Q17" s="4">
         <f t="shared" si="13"/>
-        <v>7.9360664971300459</v>
+        <v>7.6562117070496454</v>
       </c>
       <c r="R17" s="4">
         <f t="shared" si="9"/>
-        <v>8.0873944421751389</v>
+        <v>8.1208530409603146</v>
       </c>
       <c r="S17" s="4">
         <f t="shared" si="10"/>
-        <v>8.2783392676610372</v>
+        <v>8.5353535699219059</v>
       </c>
       <c r="U17">
         <v>40</v>
       </c>
-      <c r="V17" s="6" cm="1">
+      <c r="V17" s="5" cm="1">
         <f t="array" ref="V17">SUMPRODUCT(($B$35-B17) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G17</f>
-        <v>20760.08200795349</v>
-      </c>
-      <c r="W17" s="6" cm="1">
+        <v>23497.793907388601</v>
+      </c>
+      <c r="W17" s="5" cm="1">
         <f t="array" ref="W17">SUMPRODUCT(($B$35-C17) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H17</f>
-        <v>21495.722616309242</v>
-      </c>
-      <c r="X17" s="6" cm="1">
+        <v>23070.913991009766</v>
+      </c>
+      <c r="X17" s="5" cm="1">
         <f t="array" ref="X17">SUMPRODUCT(($B$35-D17) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I17</f>
-        <v>21747.547090960805</v>
+        <v>22487.710063895182</v>
       </c>
       <c r="Z17">
         <v>40</v>
       </c>
-      <c r="AA17" s="6" cm="1">
+      <c r="AA17" s="5" cm="1">
         <f t="array" ref="AA17">SUMPRODUCT(($B$35-B17) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G17</f>
-        <v>69017.164571313187</v>
-      </c>
-      <c r="AB17" s="6" cm="1">
+        <v>76431.229261138724</v>
+      </c>
+      <c r="AB17" s="5" cm="1">
         <f t="array" ref="AB17">SUMPRODUCT(($B$35-C17) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H17</f>
-        <v>72350.362344020105</v>
-      </c>
-      <c r="AC17" s="6" cm="1">
+        <v>77868.496444060191</v>
+      </c>
+      <c r="AC17" s="5" cm="1">
         <f t="array" ref="AC17">SUMPRODUCT(($B$35-D17) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I17</f>
-        <v>74389.445357708057</v>
+        <v>78695.958256481244</v>
       </c>
     </row>
     <row r="18" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -2295,88 +2300,88 @@
         <v>50</v>
       </c>
       <c r="B18">
-        <v>335.44302617197502</v>
+        <v>174.380955713779</v>
       </c>
       <c r="C18">
-        <v>248.55994698239701</v>
+        <v>114.727402038639</v>
       </c>
       <c r="D18">
-        <v>190.785787914954</v>
+        <v>69.708048419353403</v>
       </c>
       <c r="F18">
         <v>50</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="7">
         <f t="shared" si="11"/>
-        <v>15200</v>
-      </c>
-      <c r="H18">
+        <v>15947</v>
+      </c>
+      <c r="H18" s="7">
         <f t="shared" si="11"/>
-        <v>16400</v>
-      </c>
-      <c r="I18">
+        <v>17763</v>
+      </c>
+      <c r="I18" s="7">
         <f t="shared" si="11"/>
-        <v>17480</v>
+        <v>19397.400000000001</v>
       </c>
       <c r="K18">
         <v>50</v>
       </c>
-      <c r="L18" s="2">
+      <c r="L18" s="6">
         <f t="shared" si="12"/>
-        <v>0.10089190617289638</v>
-      </c>
-      <c r="M18" s="2">
+        <v>0.10626569538384781</v>
+      </c>
+      <c r="M18" s="6">
         <f t="shared" si="7"/>
-        <v>9.8807320305951407E-2</v>
-      </c>
-      <c r="N18" s="2">
+        <v>9.875992782533137E-2</v>
+      </c>
+      <c r="N18" s="6">
         <f t="shared" si="8"/>
-        <v>9.6007678036901953E-2</v>
+        <v>9.2759439490892923E-2</v>
       </c>
       <c r="P18">
         <v>50</v>
       </c>
       <c r="Q18" s="4">
         <f t="shared" si="13"/>
-        <v>8.0322330149786598</v>
+        <v>7.7036445265718001</v>
       </c>
       <c r="R18" s="4">
         <f t="shared" si="9"/>
-        <v>8.1675108385367459</v>
+        <v>8.1706403029656265</v>
       </c>
       <c r="S18" s="4">
         <f t="shared" si="10"/>
-        <v>8.3566668448076307</v>
+        <v>8.5876422211986263</v>
       </c>
       <c r="U18">
         <v>50</v>
       </c>
-      <c r="V18" s="6" cm="1">
+      <c r="V18" s="5" cm="1">
         <f t="array" ref="V18">SUMPRODUCT(($B$35-B18) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G18</f>
-        <v>20224.325973073275</v>
-      </c>
-      <c r="W18" s="6" cm="1">
+        <v>23197.771566670795</v>
+      </c>
+      <c r="W18" s="5" cm="1">
         <f t="array" ref="W18">SUMPRODUCT(($B$35-C18) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H18</f>
-        <v>21031.277505544407</v>
-      </c>
-      <c r="X18" s="6" cm="1">
+        <v>22759.735976799944</v>
+      </c>
+      <c r="X18" s="5" cm="1">
         <f t="array" ref="X18">SUMPRODUCT(($B$35-D18) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I18</f>
-        <v>21285.828929816955</v>
+        <v>22165.258382633867</v>
       </c>
       <c r="Z18">
         <v>50</v>
       </c>
-      <c r="AA18" s="6" cm="1">
+      <c r="AA18" s="5" cm="1">
         <f t="array" ref="AA18">SUMPRODUCT(($B$35-B18) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G18</f>
-        <v>67762.444013401167</v>
-      </c>
-      <c r="AB18" s="6" cm="1">
+        <v>75728.588181574072</v>
+      </c>
+      <c r="AB18" s="5" cm="1">
         <f t="array" ref="AB18">SUMPRODUCT(($B$35-C18) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H18</f>
-        <v>71262.649298233053</v>
-      </c>
-      <c r="AC18" s="6" cm="1">
+        <v>77139.729195201129</v>
+      </c>
+      <c r="AC18" s="5" cm="1">
         <f t="array" ref="AC18">SUMPRODUCT(($B$35-D18) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I18</f>
-        <v>73308.118725749446</v>
+        <v>77940.788501832896</v>
       </c>
     </row>
     <row r="19" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -2384,88 +2389,88 @@
         <v>60</v>
       </c>
       <c r="B19">
-        <v>372.76243824518002</v>
+        <v>197.67587520085499</v>
       </c>
       <c r="C19">
-        <v>281.17963178988902</v>
+        <v>134.84448259786001</v>
       </c>
       <c r="D19">
-        <v>219.43849980248399</v>
+        <v>91.036968507975303</v>
       </c>
       <c r="F19">
         <v>60</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="7">
         <f t="shared" si="11"/>
-        <v>15200</v>
-      </c>
-      <c r="H19">
+        <v>15947</v>
+      </c>
+      <c r="H19" s="7">
         <f t="shared" si="11"/>
-        <v>16400</v>
-      </c>
-      <c r="I19">
+        <v>17763</v>
+      </c>
+      <c r="I19" s="7">
         <f t="shared" si="11"/>
-        <v>17480</v>
+        <v>19397.400000000001</v>
       </c>
       <c r="K19">
         <v>60</v>
       </c>
-      <c r="L19" s="2">
+      <c r="L19" s="6">
         <f t="shared" si="12"/>
-        <v>9.8436681694396053E-2</v>
-      </c>
-      <c r="M19" s="2">
+        <v>0.10480492411106447</v>
+      </c>
+      <c r="M19" s="6">
         <f t="shared" si="7"/>
-        <v>9.6818315134762856E-2</v>
-      </c>
-      <c r="N19" s="2">
+        <v>9.7627400630644595E-2</v>
+      </c>
+      <c r="N19" s="6">
         <f t="shared" si="8"/>
-        <v>9.4368506876288102E-2</v>
+        <v>9.1659863254458046E-2</v>
       </c>
       <c r="P19">
         <v>60</v>
       </c>
       <c r="Q19" s="4">
         <f t="shared" si="13"/>
-        <v>8.1920504955538398</v>
+        <v>7.7902303905806214</v>
       </c>
       <c r="R19" s="4">
         <f t="shared" si="9"/>
-        <v>8.3009846772112752</v>
+        <v>8.2461577463981293</v>
       </c>
       <c r="S19" s="4">
         <f t="shared" si="10"/>
-        <v>8.4716196932484849</v>
+        <v>8.6688106418172435</v>
       </c>
       <c r="U19">
         <v>60</v>
       </c>
-      <c r="V19" s="6" cm="1">
+      <c r="V19" s="5" cm="1">
         <f t="array" ref="V19">SUMPRODUCT(($B$35-B19) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G19</f>
-        <v>19362.26799872578</v>
-      </c>
-      <c r="W19" s="6" cm="1">
+        <v>22659.671688081471</v>
+      </c>
+      <c r="W19" s="5" cm="1">
         <f t="array" ref="W19">SUMPRODUCT(($B$35-C19) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H19</f>
-        <v>20277.780656402181</v>
-      </c>
-      <c r="X19" s="6" cm="1">
+        <v>22295.042436541342</v>
+      </c>
+      <c r="X19" s="5" cm="1">
         <f t="array" ref="X19">SUMPRODUCT(($B$35-D19) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I19</f>
-        <v>20623.966981915015</v>
+        <v>21672.572013123281</v>
       </c>
       <c r="Z19">
         <v>60</v>
       </c>
-      <c r="AA19" s="6" cm="1">
+      <c r="AA19" s="5" cm="1">
         <f t="array" ref="AA19">SUMPRODUCT(($B$35-B19) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G19</f>
-        <v>65743.536540398782</v>
-      </c>
-      <c r="AB19" s="6" cm="1">
+        <v>74468.378429523524</v>
+      </c>
+      <c r="AB19" s="5" cm="1">
         <f t="array" ref="AB19">SUMPRODUCT(($B$35-C19) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H19</f>
-        <v>69497.987912473633</v>
-      </c>
-      <c r="AC19" s="6" cm="1">
+        <v>76051.43433684879</v>
+      </c>
+      <c r="AC19" s="5" cm="1">
         <f t="array" ref="AC19">SUMPRODUCT(($B$35-D19) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I19</f>
-        <v>71758.062844964224</v>
+        <v>76786.935486315895</v>
       </c>
     </row>
     <row r="20" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -2473,88 +2478,88 @@
         <v>70</v>
       </c>
       <c r="B20">
-        <v>431.06280760341298</v>
+        <v>237.051105197174</v>
       </c>
       <c r="C20">
-        <v>331.28572573624098</v>
+        <v>165.39215996985001</v>
       </c>
       <c r="D20">
-        <v>264.57486354943899</v>
+        <v>119.121138738566</v>
       </c>
       <c r="F20">
         <v>70</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="7">
         <f t="shared" si="11"/>
-        <v>15200</v>
-      </c>
-      <c r="H20">
+        <v>15947</v>
+      </c>
+      <c r="H20" s="7">
         <f t="shared" si="11"/>
-        <v>16400</v>
-      </c>
-      <c r="I20">
+        <v>17763</v>
+      </c>
+      <c r="I20" s="7">
         <f t="shared" si="11"/>
-        <v>17480</v>
+        <v>19397.400000000001</v>
       </c>
       <c r="K20">
         <v>70</v>
       </c>
-      <c r="L20" s="2">
+      <c r="L20" s="6">
         <f t="shared" si="12"/>
-        <v>9.4601131078722839E-2</v>
-      </c>
-      <c r="M20" s="2">
+        <v>0.10233579324028508</v>
+      </c>
+      <c r="M20" s="6">
         <f t="shared" si="7"/>
-        <v>9.3763065503887744E-2</v>
-      </c>
-      <c r="N20" s="2">
+        <v>9.5907664247601748E-2</v>
+      </c>
+      <c r="N20" s="6">
         <f t="shared" si="8"/>
-        <v>9.1786335037217448E-2</v>
+        <v>9.0212031574408616E-2</v>
       </c>
       <c r="P20">
         <v>70</v>
       </c>
       <c r="Q20" s="4">
         <f t="shared" si="13"/>
-        <v>8.4551101401816062</v>
+        <v>7.9411746959495613</v>
       </c>
       <c r="R20" s="4">
         <f t="shared" si="9"/>
-        <v>8.514898243982099</v>
+        <v>8.3635895306646084</v>
       </c>
       <c r="S20" s="4">
         <f t="shared" si="10"/>
-        <v>8.6593951570639973</v>
+        <v>8.7781061385154722</v>
       </c>
       <c r="U20">
         <v>70</v>
       </c>
-      <c r="V20" s="6" cm="1">
+      <c r="V20" s="5" cm="1">
         <f t="array" ref="V20">SUMPRODUCT(($B$35-B20) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G20</f>
-        <v>18015.561405007655</v>
-      </c>
-      <c r="W20" s="6" cm="1">
+        <v>21750.12544594051</v>
+      </c>
+      <c r="W20" s="5" cm="1">
         <f t="array" ref="W20">SUMPRODUCT(($B$35-C20) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H20</f>
-        <v>19120.357335661538</v>
-      </c>
-      <c r="X20" s="6" cm="1">
+        <v>21589.407824059708</v>
+      </c>
+      <c r="X20" s="5" cm="1">
         <f t="array" ref="X20">SUMPRODUCT(($B$35-D20) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I20</f>
-        <v>19581.341706233121</v>
+        <v>21023.843066034751</v>
       </c>
       <c r="Z20">
         <v>70</v>
       </c>
-      <c r="AA20" s="6" cm="1">
+      <c r="AA20" s="5" cm="1">
         <f t="array" ref="AA20">SUMPRODUCT(($B$35-B20) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G20</f>
-        <v>62589.600161517694</v>
-      </c>
-      <c r="AB20" s="6" cm="1">
+        <v>72338.255212822784</v>
+      </c>
+      <c r="AB20" s="5" cm="1">
         <f t="array" ref="AB20">SUMPRODUCT(($B$35-C20) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H20</f>
-        <v>66787.345866108706</v>
-      </c>
-      <c r="AC20" s="6" cm="1">
+        <v>74398.864515861249</v>
+      </c>
+      <c r="AC20" s="5" cm="1">
         <f t="array" ref="AC20">SUMPRODUCT(($B$35-D20) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I20</f>
-        <v>69316.273518430084</v>
+        <v>75267.636601317645</v>
       </c>
     </row>
     <row r="21" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -2631,88 +2636,88 @@
         <v>0</v>
       </c>
       <c r="B23">
-        <v>1079.2965670645001</v>
+        <v>855.34143228675703</v>
       </c>
       <c r="C23">
-        <v>1018.07782436601</v>
+        <v>799.22015711341101</v>
       </c>
       <c r="D23">
-        <v>967.90829483211996</v>
+        <v>752.28138598229395</v>
       </c>
       <c r="F23">
         <v>0</v>
       </c>
-      <c r="G23" s="5">
+      <c r="G23" s="8">
         <f>$B$21*$B$32+$B$34*G$12</f>
-        <v>5400</v>
-      </c>
-      <c r="H23" s="5">
+        <v>8172</v>
+      </c>
+      <c r="H23" s="8">
         <f t="shared" ref="H23:I23" si="14">$B$21*$B$32+$B$34*H$12</f>
-        <v>6600</v>
-      </c>
-      <c r="I23" s="5">
+        <v>9988</v>
+      </c>
+      <c r="I23" s="8">
         <f t="shared" si="14"/>
-        <v>7680</v>
+        <v>11622.400000000001</v>
       </c>
       <c r="K23">
         <v>0</v>
       </c>
-      <c r="L23" s="2">
+      <c r="L23" s="6">
         <f>($B$35-B23)/G23</f>
-        <v>0.14624137646953703</v>
-      </c>
-      <c r="M23" s="2">
+        <v>0.1240404512620219</v>
+      </c>
+      <c r="M23" s="6">
         <f t="shared" ref="M23:M30" si="15">($B$35-C23)/H23</f>
-        <v>0.12892760236878636</v>
-      </c>
-      <c r="N23" s="2">
+        <v>0.10710651210318271</v>
+      </c>
+      <c r="N23" s="6">
         <f t="shared" ref="N23:N30" si="16">($B$35-D23)/I23</f>
-        <v>0.11732964911040104</v>
+        <v>9.6083305859177598E-2</v>
       </c>
       <c r="P23">
         <v>0</v>
       </c>
       <c r="Q23" s="4">
         <f>LN(1+(G23*$B$36/($B$35-B23)))/LN(1+$B$36)</f>
-        <v>5.9123910814362599</v>
+        <v>6.7875968445797739</v>
       </c>
       <c r="R23" s="4">
         <f t="shared" ref="R23:R30" si="17">LN(1+(H23*$B$36/($B$35-C23)))/LN(1+$B$36)</f>
-        <v>6.5731414236558479</v>
+        <v>7.6546869998042766</v>
       </c>
       <c r="S23" s="4">
         <f t="shared" ref="S23:S30" si="18">LN(1+(I23*$B$36/($B$35-D23)))/LN(1+$B$36)</f>
-        <v>7.1062763058603258</v>
+        <v>8.3514398393359706</v>
       </c>
       <c r="U23">
         <v>0</v>
       </c>
-      <c r="V23" s="6" cm="1">
+      <c r="V23" s="5" cm="1">
         <f t="array" ref="V23">SUMPRODUCT(($B$35-B23) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G23</f>
-        <v>12841.716680751942</v>
-      </c>
-      <c r="W23" s="6" cm="1">
+        <v>15242.957605676329</v>
+      </c>
+      <c r="W23" s="5" cm="1">
         <f t="array" ref="W23">SUMPRODUCT(($B$35-C23) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H23</f>
-        <v>13055.836099869266</v>
-      </c>
-      <c r="X23" s="6" cm="1">
+        <v>14723.328317487976</v>
+      </c>
+      <c r="X23" s="5" cm="1">
         <f t="array" ref="X23">SUMPRODUCT(($B$35-D23) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I23</f>
-        <v>13134.724747930384</v>
+        <v>14173.188216338422</v>
       </c>
       <c r="Z23">
         <v>0</v>
       </c>
-      <c r="AA23" s="6" cm="1">
+      <c r="AA23" s="5" cm="1">
         <f t="array" ref="AA23">SUMPRODUCT(($B$35-B23) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G23</f>
-        <v>37321.416915188653</v>
-      </c>
-      <c r="AB23" s="6" cm="1">
+        <v>46664.95331037954</v>
+      </c>
+      <c r="AB23" s="5" cm="1">
         <f t="array" ref="AB23">SUMPRODUCT(($B$35-C23) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H23</f>
-        <v>39433.231605070432</v>
-      </c>
-      <c r="AC23" s="6" cm="1">
+        <v>47885.004940014995</v>
+      </c>
+      <c r="AC23" s="5" cm="1">
         <f t="array" ref="AC23">SUMPRODUCT(($B$35-D23) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I23</f>
-        <v>41067.305393111383</v>
+        <v>48789.900993882926</v>
       </c>
     </row>
     <row r="24" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -2720,88 +2725,88 @@
         <v>10</v>
       </c>
       <c r="B24">
-        <v>1071.3579501229201</v>
+        <v>848.08308659747399</v>
       </c>
       <c r="C24">
-        <v>1009.6558868031</v>
+        <v>791.15732352216298</v>
       </c>
       <c r="D24">
-        <v>958.57235446906702</v>
+        <v>743.68165316403599</v>
       </c>
       <c r="F24">
         <v>10</v>
       </c>
-      <c r="G24" s="5">
+      <c r="G24" s="8">
         <f t="shared" ref="G24:I30" si="19">$B$21*$B$32+$B$34*G$12</f>
-        <v>5400</v>
-      </c>
-      <c r="H24" s="5">
+        <v>8172</v>
+      </c>
+      <c r="H24" s="8">
         <f t="shared" si="19"/>
-        <v>6600</v>
-      </c>
-      <c r="I24" s="5">
+        <v>9988</v>
+      </c>
+      <c r="I24" s="8">
         <f t="shared" si="19"/>
-        <v>7680</v>
+        <v>11622.400000000001</v>
       </c>
       <c r="K24">
         <v>10</v>
       </c>
-      <c r="L24" s="2">
+      <c r="L24" s="6">
         <f t="shared" ref="L24:L30" si="20">($B$35-B24)/G24</f>
-        <v>0.14771149071797776</v>
-      </c>
-      <c r="M24" s="2">
+        <v>0.12492864823819456</v>
+      </c>
+      <c r="M24" s="6">
         <f t="shared" si="15"/>
-        <v>0.13020365351468183</v>
-      </c>
-      <c r="N24" s="2">
+        <v>0.10791376416478143</v>
+      </c>
+      <c r="N24" s="6">
         <f t="shared" si="16"/>
-        <v>0.11854526634517357</v>
+        <v>9.6823233311189055E-2</v>
       </c>
       <c r="P24">
         <v>10</v>
       </c>
       <c r="Q24" s="4">
         <f t="shared" ref="Q24:Q30" si="21">LN(1+(G24*$B$36/($B$35-B24)))/LN(1+$B$36)</f>
-        <v>5.8624104959342009</v>
+        <v>6.7475742056393422</v>
       </c>
       <c r="R24" s="4">
         <f t="shared" si="17"/>
-        <v>6.5193849503105801</v>
+        <v>7.6082749538144947</v>
       </c>
       <c r="S24" s="4">
         <f t="shared" si="18"/>
-        <v>7.0463191720432334</v>
+        <v>8.3006491578097066</v>
       </c>
       <c r="U24">
         <v>10</v>
       </c>
-      <c r="V24" s="6" cm="1">
+      <c r="V24" s="5" cm="1">
         <f t="array" ref="V24">SUMPRODUCT(($B$35-B24) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G24</f>
-        <v>13025.094383121825</v>
-      </c>
-      <c r="W24" s="6" cm="1">
+        <v>15410.621414788413</v>
+      </c>
+      <c r="W24" s="5" cm="1">
         <f t="array" ref="W24">SUMPRODUCT(($B$35-C24) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H24</f>
-        <v>13250.378243816282</v>
-      </c>
-      <c r="X24" s="6" cm="1">
+        <v>14909.57535641608</v>
+      </c>
+      <c r="X24" s="5" cm="1">
         <f t="array" ref="X24">SUMPRODUCT(($B$35-D24) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I24</f>
-        <v>13350.379855846215</v>
+        <v>14371.837333283103</v>
       </c>
       <c r="Z24">
         <v>10</v>
       </c>
-      <c r="AA24" s="6" cm="1">
+      <c r="AA24" s="5" cm="1">
         <f t="array" ref="AA24">SUMPRODUCT(($B$35-B24) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G24</f>
-        <v>37750.880622634533</v>
-      </c>
-      <c r="AB24" s="6" cm="1">
+        <v>47057.615668644539</v>
+      </c>
+      <c r="AB24" s="5" cm="1">
         <f t="array" ref="AB24">SUMPRODUCT(($B$35-C24) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H24</f>
-        <v>39888.842016337512</v>
-      </c>
-      <c r="AC24" s="6" cm="1">
+        <v>48321.18852616084</v>
+      </c>
+      <c r="AC24" s="5" cm="1">
         <f t="array" ref="AC24">SUMPRODUCT(($B$35-D24) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I24</f>
-        <v>41572.361574851304</v>
+        <v>49255.129782014621</v>
       </c>
     </row>
     <row r="25" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -2809,88 +2814,88 @@
         <v>20</v>
       </c>
       <c r="B25">
-        <v>1071.8074857813899</v>
+        <v>848.70622853402404</v>
       </c>
       <c r="C25">
-        <v>1010.80982066353</v>
+        <v>791.99283303668096</v>
       </c>
       <c r="D25">
-        <v>959.95653000581206</v>
+        <v>744.21830838338099</v>
       </c>
       <c r="F25">
         <v>20</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G25" s="8">
         <f t="shared" si="19"/>
-        <v>5400</v>
-      </c>
-      <c r="H25" s="5">
+        <v>8172</v>
+      </c>
+      <c r="H25" s="8">
         <f t="shared" si="19"/>
-        <v>6600</v>
-      </c>
-      <c r="I25" s="5">
+        <v>9988</v>
+      </c>
+      <c r="I25" s="8">
         <f t="shared" si="19"/>
-        <v>7680</v>
+        <v>11622.400000000001</v>
       </c>
       <c r="K25">
         <v>20</v>
       </c>
-      <c r="L25" s="2">
+      <c r="L25" s="6">
         <f t="shared" si="20"/>
-        <v>0.14762824337381669</v>
-      </c>
-      <c r="M25" s="2">
+        <v>0.12485239494199413</v>
+      </c>
+      <c r="M25" s="6">
         <f t="shared" si="15"/>
-        <v>0.1300288150509803</v>
-      </c>
-      <c r="N25" s="2">
+        <v>0.10783011283172997</v>
+      </c>
+      <c r="N25" s="6">
         <f t="shared" si="16"/>
-        <v>0.11836503515549322</v>
+        <v>9.6777059094216231E-2</v>
       </c>
       <c r="P25">
         <v>20</v>
       </c>
       <c r="Q25" s="4">
         <f t="shared" si="21"/>
-        <v>5.8652179251316143</v>
+        <v>6.7509914597141742</v>
       </c>
       <c r="R25" s="4">
         <f t="shared" si="17"/>
-        <v>6.5266977599624667</v>
+        <v>7.6130578236340289</v>
       </c>
       <c r="S25" s="4">
         <f t="shared" si="18"/>
-        <v>7.0551437716736798</v>
+        <v>8.3038002646271032</v>
       </c>
       <c r="U25">
         <v>20</v>
       </c>
-      <c r="V25" s="6" cm="1">
+      <c r="V25" s="5" cm="1">
         <f t="array" ref="V25">SUMPRODUCT(($B$35-B25) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G25</f>
-        <v>13014.710355678486</v>
-      </c>
-      <c r="W25" s="6" cm="1">
+        <v>15396.227177427452</v>
+      </c>
+      <c r="W25" s="5" cm="1">
         <f t="array" ref="W25">SUMPRODUCT(($B$35-C25) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H25</f>
-        <v>13223.723003795298</v>
-      </c>
-      <c r="X25" s="6" cm="1">
+        <v>14890.275544344528</v>
+      </c>
+      <c r="X25" s="5" cm="1">
         <f t="array" ref="X25">SUMPRODUCT(($B$35-D25) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I25</f>
-        <v>13318.406159234724</v>
+        <v>14359.440891709906</v>
       </c>
       <c r="Z25">
         <v>20</v>
       </c>
-      <c r="AA25" s="6" cm="1">
+      <c r="AA25" s="5" cm="1">
         <f t="array" ref="AA25">SUMPRODUCT(($B$35-B25) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G25</f>
-        <v>37726.561619471111</v>
-      </c>
-      <c r="AB25" s="6" cm="1">
+        <v>47023.904904124072</v>
+      </c>
+      <c r="AB25" s="5" cm="1">
         <f t="array" ref="AB25">SUMPRODUCT(($B$35-C25) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H25</f>
-        <v>39826.416443029913</v>
-      </c>
-      <c r="AC25" s="6" cm="1">
+        <v>48275.989089489223</v>
+      </c>
+      <c r="AC25" s="5" cm="1">
         <f t="array" ref="AC25">SUMPRODUCT(($B$35-D25) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I25</f>
-        <v>41497.480375501218</v>
+        <v>49226.097780367971</v>
       </c>
     </row>
     <row r="26" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -2898,88 +2903,88 @@
         <v>30</v>
       </c>
       <c r="B26">
-        <v>1078.6432326015399</v>
+        <v>855.10775863383697</v>
       </c>
       <c r="C26">
-        <v>1019.1387802197499</v>
+        <v>799.58687820807097</v>
       </c>
       <c r="D26">
-        <v>969.34202963804296</v>
+        <v>752.59055372453702</v>
       </c>
       <c r="F26">
         <v>30</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G26" s="8">
         <f t="shared" si="19"/>
-        <v>5400</v>
-      </c>
-      <c r="H26" s="5">
+        <v>8172</v>
+      </c>
+      <c r="H26" s="8">
         <f t="shared" si="19"/>
-        <v>6600</v>
-      </c>
-      <c r="I26" s="5">
+        <v>9988</v>
+      </c>
+      <c r="I26" s="8">
         <f t="shared" si="19"/>
-        <v>7680</v>
+        <v>11622.400000000001</v>
       </c>
       <c r="K26">
         <v>30</v>
       </c>
-      <c r="L26" s="2">
+      <c r="L26" s="6">
         <f t="shared" si="20"/>
-        <v>0.14636236433304817</v>
-      </c>
-      <c r="M26" s="2">
+        <v>0.12406904568846831</v>
+      </c>
+      <c r="M26" s="6">
         <f t="shared" si="15"/>
-        <v>0.12876685148185607</v>
-      </c>
-      <c r="N26" s="2">
+        <v>0.10706979593431407</v>
+      </c>
+      <c r="N26" s="6">
         <f t="shared" si="16"/>
-        <v>0.11714296489087982</v>
+        <v>9.6056704835099704E-2</v>
       </c>
       <c r="P26">
         <v>30</v>
       </c>
       <c r="Q26" s="4">
         <f t="shared" si="21"/>
-        <v>5.9082452988619485</v>
+        <v>6.7863008760791095</v>
       </c>
       <c r="R26" s="4">
         <f t="shared" si="17"/>
-        <v>6.5799770934996857</v>
+        <v>7.6568116367071815</v>
       </c>
       <c r="S26" s="4">
         <f t="shared" si="18"/>
-        <v>7.1155757658924932</v>
+        <v>8.3532776052349984</v>
       </c>
       <c r="U26">
         <v>30</v>
       </c>
-      <c r="V26" s="6" cm="1">
+      <c r="V26" s="5" cm="1">
         <f t="array" ref="V26">SUMPRODUCT(($B$35-B26) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G26</f>
-        <v>12856.808348932733</v>
-      </c>
-      <c r="W26" s="6" cm="1">
+        <v>15248.355339046284</v>
+      </c>
+      <c r="W26" s="5" cm="1">
         <f t="array" ref="W26">SUMPRODUCT(($B$35-C26) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H26</f>
-        <v>13031.328600867062</v>
-      </c>
-      <c r="X26" s="6" cm="1">
+        <v>14714.857261100668</v>
+      </c>
+      <c r="X26" s="5" cm="1">
         <f t="array" ref="X26">SUMPRODUCT(($B$35-D26) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I26</f>
-        <v>13101.606259350738</v>
+        <v>14166.046610862726</v>
       </c>
       <c r="Z26">
         <v>30</v>
       </c>
-      <c r="AA26" s="6" cm="1">
+      <c r="AA26" s="5" cm="1">
         <f t="array" ref="AA26">SUMPRODUCT(($B$35-B26) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G26</f>
-        <v>37356.761036555115</v>
-      </c>
-      <c r="AB26" s="6" cm="1">
+        <v>46677.594599668839</v>
+      </c>
+      <c r="AB26" s="5" cm="1">
         <f t="array" ref="AB26">SUMPRODUCT(($B$35-C26) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H26</f>
-        <v>39375.835960748933</v>
-      </c>
-      <c r="AC26" s="6" cm="1">
+        <v>47865.166043382211</v>
+      </c>
+      <c r="AC26" s="5" cm="1">
         <f t="array" ref="AC26">SUMPRODUCT(($B$35-D26) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I26</f>
-        <v>40989.74313386935</v>
+        <v>48773.175621468115</v>
       </c>
     </row>
     <row r="27" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -2987,88 +2992,88 @@
         <v>40</v>
       </c>
       <c r="B27">
-        <v>1092.5747991635001</v>
+        <v>867.22096553860104</v>
       </c>
       <c r="C27">
-        <v>1034.84553978592</v>
+        <v>813.73079032396697</v>
       </c>
       <c r="D27">
-        <v>986.525066375336</v>
+        <v>768.28093879695302</v>
       </c>
       <c r="F27">
         <v>40</v>
       </c>
-      <c r="G27" s="5">
+      <c r="G27" s="8">
         <f t="shared" si="19"/>
-        <v>5400</v>
-      </c>
-      <c r="H27" s="5">
+        <v>8172</v>
+      </c>
+      <c r="H27" s="8">
         <f t="shared" si="19"/>
-        <v>6600</v>
-      </c>
-      <c r="I27" s="5">
+        <v>9988</v>
+      </c>
+      <c r="I27" s="8">
         <f t="shared" si="19"/>
-        <v>7680</v>
+        <v>11622.400000000001</v>
       </c>
       <c r="K27">
         <v>40</v>
       </c>
-      <c r="L27" s="2">
+      <c r="L27" s="6">
         <f t="shared" si="20"/>
-        <v>0.14378244459935183</v>
-      </c>
-      <c r="M27" s="2">
+        <v>0.12258676388416531</v>
+      </c>
+      <c r="M27" s="6">
         <f t="shared" si="15"/>
-        <v>0.12638703942637575</v>
-      </c>
-      <c r="N27" s="2">
+        <v>0.10565370541410021</v>
+      </c>
+      <c r="N27" s="6">
         <f t="shared" si="16"/>
-        <v>0.11490559031571146</v>
+        <v>9.4706692352960392E-2</v>
       </c>
       <c r="P27">
         <v>40</v>
       </c>
       <c r="Q27" s="4">
         <f t="shared" si="21"/>
-        <v>5.9979406459358824</v>
+        <v>6.8541485374859343</v>
       </c>
       <c r="R27" s="4">
         <f t="shared" si="17"/>
-        <v>6.6828845913806729</v>
+        <v>7.7396804493760492</v>
       </c>
       <c r="S27" s="4">
         <f t="shared" si="18"/>
-        <v>7.2289794777291823</v>
+        <v>8.447639979047592</v>
       </c>
       <c r="U27">
         <v>40</v>
       </c>
-      <c r="V27" s="6" cm="1">
+      <c r="V27" s="5" cm="1">
         <f t="array" ref="V27">SUMPRODUCT(($B$35-B27) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G27</f>
-        <v>12534.996793425576</v>
-      </c>
-      <c r="W27" s="6" cm="1">
+        <v>14968.546895475694</v>
+      </c>
+      <c r="W27" s="5" cm="1">
         <f t="array" ref="W27">SUMPRODUCT(($B$35-C27) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H27</f>
-        <v>12668.511059459506</v>
-      </c>
-      <c r="X27" s="6" cm="1">
+        <v>14388.140639626006</v>
+      </c>
+      <c r="X27" s="5" cm="1">
         <f t="array" ref="X27">SUMPRODUCT(($B$35-D27) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I27</f>
-        <v>12704.68752403323</v>
+        <v>13803.607311290514</v>
       </c>
       <c r="Z27">
         <v>40</v>
       </c>
-      <c r="AA27" s="6" cm="1">
+      <c r="AA27" s="5" cm="1">
         <f t="array" ref="AA27">SUMPRODUCT(($B$35-B27) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G27</f>
-        <v>36603.090432436285</v>
-      </c>
-      <c r="AB27" s="6" cm="1">
+        <v>46022.293709770551</v>
+      </c>
+      <c r="AB27" s="5" cm="1">
         <f t="array" ref="AB27">SUMPRODUCT(($B$35-C27) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H27</f>
-        <v>38526.130874222123</v>
-      </c>
-      <c r="AC27" s="6" cm="1">
+        <v>47100.007958569448</v>
+      </c>
+      <c r="AC27" s="5" cm="1">
         <f t="array" ref="AC27">SUMPRODUCT(($B$35-D27) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I27</f>
-        <v>40060.174329040747</v>
+        <v>47924.35636314626</v>
       </c>
     </row>
     <row r="28" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -3076,88 +3081,88 @@
         <v>50</v>
       </c>
       <c r="B28">
-        <v>1112.6919986630701</v>
+        <v>884.72312853946801</v>
       </c>
       <c r="C28">
-        <v>1057.0230347209799</v>
+        <v>833.45672586742899</v>
       </c>
       <c r="D28">
-        <v>1010.53788541441</v>
+        <v>790.03783874614498</v>
       </c>
       <c r="F28">
         <v>50</v>
       </c>
-      <c r="G28" s="5">
+      <c r="G28" s="8">
         <f t="shared" si="19"/>
-        <v>5400</v>
-      </c>
-      <c r="H28" s="5">
+        <v>8172</v>
+      </c>
+      <c r="H28" s="8">
         <f t="shared" si="19"/>
-        <v>6600</v>
-      </c>
-      <c r="I28" s="5">
+        <v>9988</v>
+      </c>
+      <c r="I28" s="8">
         <f t="shared" si="19"/>
-        <v>7680</v>
+        <v>11622.400000000001</v>
       </c>
       <c r="K28">
         <v>50</v>
       </c>
-      <c r="L28" s="2">
+      <c r="L28" s="6">
         <f t="shared" si="20"/>
-        <v>0.14005703728461666</v>
-      </c>
-      <c r="M28" s="2">
+        <v>0.12044504056051542</v>
+      </c>
+      <c r="M28" s="6">
         <f t="shared" si="15"/>
-        <v>0.12302681292106364</v>
-      </c>
-      <c r="N28" s="2">
+        <v>0.10367874190354136</v>
+      </c>
+      <c r="N28" s="6">
         <f t="shared" si="16"/>
-        <v>0.1117789211699987</v>
+        <v>9.2834712387618284E-2</v>
       </c>
       <c r="P28">
         <v>50</v>
       </c>
       <c r="Q28" s="4">
         <f t="shared" si="21"/>
-        <v>6.1324246981848267</v>
+        <v>6.9546439259745343</v>
       </c>
       <c r="R28" s="4">
         <f t="shared" si="17"/>
-        <v>6.8338634427718317</v>
+        <v>7.8583467215669032</v>
       </c>
       <c r="S28" s="4">
         <f t="shared" si="18"/>
-        <v>7.3937438533429027</v>
+        <v>8.5821424018752097</v>
       </c>
       <c r="U28">
         <v>50</v>
       </c>
-      <c r="V28" s="6" cm="1">
+      <c r="V28" s="5" cm="1">
         <f t="array" ref="V28">SUMPRODUCT(($B$35-B28) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G28</f>
-        <v>12070.300505710067</v>
-      </c>
-      <c r="W28" s="6" cm="1">
+        <v>14564.256518295286</v>
+      </c>
+      <c r="W28" s="5" cm="1">
         <f t="array" ref="W28">SUMPRODUCT(($B$35-C28) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H28</f>
-        <v>12156.223075867547</v>
-      </c>
-      <c r="X28" s="6" cm="1">
+        <v>13932.482334952034</v>
+      </c>
+      <c r="X28" s="5" cm="1">
         <f t="array" ref="X28">SUMPRODUCT(($B$35-D28) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I28</f>
-        <v>12150.004559076777</v>
+        <v>13301.034841459244</v>
       </c>
       <c r="Z28">
         <v>50</v>
       </c>
-      <c r="AA28" s="6" cm="1">
+      <c r="AA28" s="5" cm="1">
         <f t="array" ref="AA28">SUMPRODUCT(($B$35-B28) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G28</f>
-        <v>35514.789139642817</v>
-      </c>
-      <c r="AB28" s="6" cm="1">
+        <v>45075.460795928193</v>
+      </c>
+      <c r="AB28" s="5" cm="1">
         <f t="array" ref="AB28">SUMPRODUCT(($B$35-C28) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H28</f>
-        <v>37326.371613035568</v>
-      </c>
-      <c r="AC28" s="6" cm="1">
+        <v>46032.873283389177</v>
+      </c>
+      <c r="AC28" s="5" cm="1">
         <f t="array" ref="AC28">SUMPRODUCT(($B$35-D28) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I28</f>
-        <v>38761.127610117539</v>
+        <v>46747.350471128826</v>
       </c>
     </row>
     <row r="29" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -3165,88 +3170,88 @@
         <v>60</v>
       </c>
       <c r="B29">
-        <v>1137.7105905984499</v>
+        <v>906.61297638021199</v>
       </c>
       <c r="C29">
-        <v>1084.3937667770199</v>
+        <v>857.76160515654897</v>
       </c>
       <c r="D29">
-        <v>1040.0231709887</v>
+        <v>816.43641321394603</v>
       </c>
       <c r="F29">
         <v>60</v>
       </c>
-      <c r="G29" s="5">
+      <c r="G29" s="8">
         <f t="shared" si="19"/>
-        <v>5400</v>
-      </c>
-      <c r="H29" s="5">
+        <v>8172</v>
+      </c>
+      <c r="H29" s="8">
         <f t="shared" si="19"/>
-        <v>6600</v>
-      </c>
-      <c r="I29" s="5">
+        <v>9988</v>
+      </c>
+      <c r="I29" s="8">
         <f t="shared" si="19"/>
-        <v>7680</v>
+        <v>11622.400000000001</v>
       </c>
       <c r="K29">
         <v>60</v>
       </c>
-      <c r="L29" s="2">
+      <c r="L29" s="6">
         <f t="shared" si="20"/>
-        <v>0.13542396470399076</v>
-      </c>
-      <c r="M29" s="2">
+        <v>0.11776640034505483</v>
+      </c>
+      <c r="M29" s="6">
         <f t="shared" si="15"/>
-        <v>0.11887973230651214</v>
-      </c>
-      <c r="N29" s="2">
+        <v>0.10124533388500712</v>
+      </c>
+      <c r="N29" s="6">
         <f t="shared" si="16"/>
-        <v>0.10793969127751302</v>
+        <v>9.0563359270551161E-2</v>
       </c>
       <c r="P29">
         <v>60</v>
       </c>
       <c r="Q29" s="4">
         <f t="shared" si="21"/>
-        <v>6.3084239453975748</v>
+        <v>7.0846160072224498</v>
       </c>
       <c r="R29" s="4">
         <f t="shared" si="17"/>
-        <v>7.0300019751615421</v>
+        <v>8.0097483508531013</v>
       </c>
       <c r="S29" s="4">
         <f t="shared" si="18"/>
-        <v>7.6067937776514869</v>
+        <v>8.7513269897393844</v>
       </c>
       <c r="U29">
         <v>60</v>
       </c>
-      <c r="V29" s="6" cm="1">
+      <c r="V29" s="5" cm="1">
         <f t="array" ref="V29">SUMPRODUCT(($B$35-B29) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G29</f>
-        <v>11492.38473783747</v>
-      </c>
-      <c r="W29" s="6" cm="1">
+        <v>14058.613025001476</v>
+      </c>
+      <c r="W29" s="5" cm="1">
         <f t="array" ref="W29">SUMPRODUCT(($B$35-C29) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H29</f>
-        <v>11523.974159771169</v>
-      </c>
-      <c r="X29" s="6" cm="1">
+        <v>13371.052938217708</v>
+      </c>
+      <c r="X29" s="5" cm="1">
         <f t="array" ref="X29">SUMPRODUCT(($B$35-D29) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I29</f>
-        <v>11468.91061511618</v>
+        <v>12691.242233078003</v>
       </c>
       <c r="Z29">
         <v>60</v>
       </c>
-      <c r="AA29" s="6" cm="1">
+      <c r="AA29" s="5" cm="1">
         <f t="array" ref="AA29">SUMPRODUCT(($B$35-B29) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G29</f>
-        <v>34161.332066866438</v>
-      </c>
-      <c r="AB29" s="6" cm="1">
+        <v>43891.262682038468</v>
+      </c>
+      <c r="AB29" s="5" cm="1">
         <f t="array" ref="AB29">SUMPRODUCT(($B$35-C29) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H29</f>
-        <v>35845.66834308346</v>
-      </c>
-      <c r="AC29" s="6" cm="1">
+        <v>44718.026674043562</v>
+      </c>
+      <c r="AC29" s="5" cm="1">
         <f t="array" ref="AC29">SUMPRODUCT(($B$35-D29) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I29</f>
-        <v>37166.031115221675</v>
+        <v>45319.23903236584</v>
       </c>
     </row>
     <row r="30" spans="1:29" ht="19" x14ac:dyDescent="0.25">
@@ -3254,88 +3259,88 @@
         <v>70</v>
       </c>
       <c r="B30">
-        <v>1167.3791554115301</v>
+        <v>932.92485462626496</v>
       </c>
       <c r="C30">
-        <v>1117.0363910849201</v>
+        <v>887.20182443517797</v>
       </c>
       <c r="D30">
-        <v>1075.3121226656201</v>
+        <v>848.62098664477401</v>
       </c>
       <c r="F30">
         <v>70</v>
       </c>
-      <c r="G30" s="5">
+      <c r="G30" s="8">
         <f t="shared" si="19"/>
-        <v>5400</v>
-      </c>
-      <c r="H30" s="5">
+        <v>8172</v>
+      </c>
+      <c r="H30" s="8">
         <f t="shared" si="19"/>
-        <v>6600</v>
-      </c>
-      <c r="I30" s="5">
+        <v>9988</v>
+      </c>
+      <c r="I30" s="8">
         <f t="shared" si="19"/>
-        <v>7680</v>
+        <v>11622.400000000001</v>
       </c>
       <c r="K30">
         <v>70</v>
       </c>
-      <c r="L30" s="2">
+      <c r="L30" s="6">
         <f t="shared" si="20"/>
-        <v>0.12992978603490185</v>
-      </c>
-      <c r="M30" s="2">
+        <v>0.11454664040305128</v>
+      </c>
+      <c r="M30" s="6">
         <f t="shared" si="15"/>
-        <v>0.11393388013864847</v>
-      </c>
-      <c r="N30" s="2">
+        <v>9.8297774886345821E-2</v>
+      </c>
+      <c r="N30" s="6">
         <f t="shared" si="16"/>
-        <v>0.10334477569458071</v>
+        <v>8.7794174469578212E-2</v>
       </c>
       <c r="P30">
         <v>70</v>
       </c>
       <c r="Q30" s="4">
         <f t="shared" si="21"/>
-        <v>6.5308471238240182</v>
+        <v>7.2475154188426538</v>
       </c>
       <c r="R30" s="4">
         <f t="shared" si="17"/>
-        <v>7.2793817604635978</v>
+        <v>8.2012861226816458</v>
       </c>
       <c r="S30" s="4">
         <f t="shared" si="18"/>
-        <v>7.8787799157066365</v>
+        <v>8.9670420607146628</v>
       </c>
       <c r="U30">
         <v>70</v>
       </c>
-      <c r="V30" s="6" cm="1">
+      <c r="V30" s="5" cm="1">
         <f t="array" ref="V30">SUMPRODUCT(($B$35-B30) * (1 + $B$36) ^ (ROW($1:$15) - 1))-G30</f>
-        <v>10807.05714386595</v>
-      </c>
-      <c r="W30" s="6" cm="1">
+        <v>13450.823051848172</v>
+      </c>
+      <c r="W30" s="5" cm="1">
         <f t="array" ref="W30">SUMPRODUCT(($B$35-C30) * (1 + $B$36) ^ (ROW($1:$15) - 1))-H30</f>
-        <v>10769.947420736371</v>
-      </c>
-      <c r="X30" s="6" cm="1">
+        <v>12691.000000998403</v>
+      </c>
+      <c r="X30" s="5" cm="1">
         <f t="array" ref="X30">SUMPRODUCT(($B$35-D30) * (1 + $B$36) ^ (ROW($1:$15) - 1))-I30</f>
-        <v>10653.755163583908</v>
+        <v>11947.796218371404</v>
       </c>
       <c r="Z30">
         <v>70</v>
       </c>
-      <c r="AA30" s="6" cm="1">
+      <c r="AA30" s="5" cm="1">
         <f t="array" ref="AA30">SUMPRODUCT(($B$35-B30) * (1 + $B$36) ^ (ROW($1:$25) - 1))-G30</f>
-        <v>32556.320522287759</v>
-      </c>
-      <c r="AB30" s="6" cm="1">
+        <v>42467.841339936829</v>
+      </c>
+      <c r="AB30" s="5" cm="1">
         <f t="array" ref="AB30">SUMPRODUCT(($B$35-C30) * (1 + $B$36) ^ (ROW($1:$25) - 1))-H30</f>
-        <v>34079.76597505161</v>
-      </c>
-      <c r="AC30" s="6" cm="1">
+        <v>43125.368177927339</v>
+      </c>
+      <c r="AC30" s="5" cm="1">
         <f t="array" ref="AC30">SUMPRODUCT(($B$35-D30) * (1 + $B$36) ^ (ROW($1:$25) - 1))-I30</f>
-        <v>35256.967593127571</v>
+        <v>43578.116324231181</v>
       </c>
     </row>
     <row r="31" spans="1:29" x14ac:dyDescent="0.2">
@@ -3348,7 +3353,7 @@
         <v>0</v>
       </c>
       <c r="B32" s="3">
-        <v>9800</v>
+        <v>7775</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
@@ -3356,7 +3361,7 @@
         <v>2</v>
       </c>
       <c r="B33" s="3">
-        <v>1.2</v>
+        <v>1.8160000000000001</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
@@ -3365,7 +3370,7 @@
       </c>
       <c r="B34" s="3">
         <f>B33*1000</f>
-        <v>1200</v>
+        <v>1816</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
@@ -3394,8 +3399,20 @@
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="B13:D20 B23:D30">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="G3:I10">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3407,7 +3424,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G13:I21 G23:I30">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3419,7 +3436,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L3:N10">
-    <cfRule type="colorScale" priority="15">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3430,8 +3447,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L13:N21 L23:N30">
-    <cfRule type="colorScale" priority="14">
+  <conditionalFormatting sqref="L13:N20">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L23:N30">
+    <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3443,7 +3472,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q3:S10">
-    <cfRule type="colorScale" priority="11">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3455,7 +3484,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q13:S21 Q23:S30">
-    <cfRule type="colorScale" priority="10">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3467,7 +3496,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V23:X30 V13:X20 V3:X10">
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="8">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3479,7 +3508,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA3:AC10 AA13:AC20 AA23:AC30">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>